<commit_message>
update CCHF, Nipah AI checked file, in the future all the intermediate files wont be saved in this repo
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E355233-A3BF-834A-B1C3-78B443EE492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3044545F-6BBC-CD43-9A12-8B35470DB7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="500" windowWidth="35680" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="1120" windowWidth="35680" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="511">
   <si>
     <t>RefID</t>
   </si>
@@ -1721,6 +1721,21 @@
   </si>
   <si>
     <t>Double check</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijid.2023.04.042</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijid.2012.05.899</t>
+  </si>
+  <si>
+    <t>10.18678/dtfd.864114</t>
+  </si>
+  <si>
+    <t>10.15690/vramn1192</t>
+  </si>
+  <si>
+    <t>32655079, 26902209</t>
   </si>
 </sst>
 </file>
@@ -2128,10 +2143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2172,7 +2188,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2199,7 +2215,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2223,7 +2239,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2250,7 +2266,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2298,7 +2314,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2322,7 +2338,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -2351,7 +2367,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -2378,7 +2394,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
@@ -2402,7 +2418,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -2426,7 +2442,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
@@ -2450,7 +2466,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>26</v>
       </c>
@@ -2474,7 +2490,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>27</v>
       </c>
@@ -2503,7 +2519,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="304" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="304" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>31</v>
       </c>
@@ -2530,7 +2546,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>33</v>
       </c>
@@ -2554,7 +2570,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>34</v>
       </c>
@@ -2578,7 +2594,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>35</v>
       </c>
@@ -2602,7 +2618,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>36</v>
       </c>
@@ -2626,7 +2642,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>37</v>
       </c>
@@ -2650,7 +2666,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>38</v>
       </c>
@@ -2674,7 +2690,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>39</v>
       </c>
@@ -2695,7 +2711,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>43</v>
       </c>
@@ -2719,7 +2735,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>48</v>
       </c>
@@ -2743,7 +2759,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>52</v>
       </c>
@@ -2767,7 +2783,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>54</v>
       </c>
@@ -2791,7 +2807,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>57</v>
       </c>
@@ -2820,7 +2836,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>62</v>
       </c>
@@ -2839,7 +2855,9 @@
       <c r="F28" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="H28" s="5" t="s">
         <v>123</v>
       </c>
@@ -2847,7 +2865,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>63</v>
       </c>
@@ -2871,7 +2889,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="320" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>64</v>
       </c>
@@ -2900,7 +2918,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="365" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="365" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>67</v>
       </c>
@@ -2929,7 +2947,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>68</v>
       </c>
@@ -2953,7 +2971,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>70</v>
       </c>
@@ -2982,7 +3000,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>71</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>72</v>
       </c>
@@ -3040,7 +3058,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>76</v>
       </c>
@@ -3064,7 +3082,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>84</v>
       </c>
@@ -3091,7 +3109,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>102</v>
       </c>
@@ -3120,7 +3138,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="304" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="304" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>106</v>
       </c>
@@ -3147,7 +3165,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>108</v>
       </c>
@@ -3174,7 +3192,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>109</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>110</v>
       </c>
@@ -3230,7 +3248,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>113</v>
       </c>
@@ -3249,7 +3267,9 @@
       <c r="F43" t="s">
         <v>205</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="H43" s="5" t="s">
         <v>454</v>
       </c>
@@ -3257,7 +3277,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>116</v>
       </c>
@@ -3281,7 +3301,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>117</v>
       </c>
@@ -3305,7 +3325,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>118</v>
       </c>
@@ -3334,7 +3354,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>120</v>
       </c>
@@ -3363,7 +3383,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>123</v>
       </c>
@@ -3392,7 +3412,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>125</v>
       </c>
@@ -3421,7 +3441,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="320" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>132</v>
       </c>
@@ -3448,7 +3468,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>142</v>
       </c>
@@ -3472,7 +3492,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>144</v>
       </c>
@@ -3496,7 +3516,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>145</v>
       </c>
@@ -3520,7 +3540,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>146</v>
       </c>
@@ -3547,7 +3567,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>147</v>
       </c>
@@ -3574,7 +3594,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>148</v>
       </c>
@@ -3603,7 +3623,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>152</v>
       </c>
@@ -3622,12 +3642,14 @@
       <c r="F57" t="s">
         <v>292</v>
       </c>
-      <c r="G57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="H57" s="5" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>153</v>
       </c>
@@ -3651,7 +3673,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>155</v>
       </c>
@@ -3670,12 +3692,14 @@
       <c r="F59" t="s">
         <v>301</v>
       </c>
-      <c r="G59" s="2"/>
+      <c r="G59" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="H59" s="5" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>157</v>
       </c>
@@ -3704,7 +3728,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>159</v>
       </c>
@@ -3728,7 +3752,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>160</v>
       </c>
@@ -3757,7 +3781,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>162</v>
       </c>
@@ -3781,7 +3805,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>170</v>
       </c>
@@ -3810,7 +3834,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="335" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="335" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>174</v>
       </c>
@@ -3837,7 +3861,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>177</v>
       </c>
@@ -3866,7 +3890,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>180</v>
       </c>
@@ -3890,7 +3914,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>182</v>
       </c>
@@ -3914,7 +3938,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>185</v>
       </c>
@@ -3943,7 +3967,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>186</v>
       </c>
@@ -3989,7 +4013,9 @@
       <c r="F71" t="s">
         <v>363</v>
       </c>
-      <c r="G71" s="2"/>
+      <c r="G71" s="2" t="s">
+        <v>510</v>
+      </c>
       <c r="H71" s="5" t="s">
         <v>491</v>
       </c>
@@ -3997,7 +4023,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>190</v>
       </c>
@@ -4024,7 +4050,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>191</v>
       </c>
@@ -4048,7 +4074,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>192</v>
       </c>
@@ -4077,7 +4103,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>194</v>
       </c>
@@ -4106,7 +4132,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>195</v>
       </c>
@@ -4133,7 +4159,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>197</v>
       </c>
@@ -4162,7 +4188,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>204</v>
       </c>
@@ -4186,7 +4212,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>208</v>
       </c>
@@ -4210,7 +4236,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>11</v>
       </c>
@@ -4236,7 +4262,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>13</v>
       </c>
@@ -4265,7 +4291,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="256" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>23</v>
       </c>
@@ -4294,7 +4320,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>28</v>
       </c>
@@ -4320,7 +4346,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>30</v>
       </c>
@@ -4349,7 +4375,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>32</v>
       </c>
@@ -4378,7 +4404,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="320" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>41</v>
       </c>
@@ -4407,7 +4433,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>47</v>
       </c>
@@ -4433,7 +4459,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="335" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="335" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>55</v>
       </c>
@@ -4462,7 +4488,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>73</v>
       </c>
@@ -4491,7 +4517,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>82</v>
       </c>
@@ -4520,7 +4546,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>87</v>
       </c>
@@ -4549,7 +4575,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>112</v>
       </c>
@@ -4578,7 +4604,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>114</v>
       </c>
@@ -4607,7 +4633,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>119</v>
       </c>
@@ -4636,7 +4662,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>126</v>
       </c>
@@ -4665,7 +4691,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>129</v>
       </c>
@@ -4694,7 +4720,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>131</v>
       </c>
@@ -4723,7 +4749,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>140</v>
       </c>
@@ -4752,7 +4778,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>158</v>
       </c>
@@ -4781,7 +4807,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>166</v>
       </c>
@@ -4807,7 +4833,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>173</v>
       </c>
@@ -4837,7 +4863,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I101" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="188"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fix submission set author order
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBA0D2-56FB-4446-99B1-CD83E472DA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99078FD1-2B2B-AB4B-ABF3-85FFA437D69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="500" windowWidth="35560" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="500" windowWidth="25740" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,9 +227,6 @@
     <t>Genotypes of the congo-crimean hemorrhagic fever virus occurring in the turkestan region</t>
   </si>
   <si>
-    <t>Abuova G., Aliyev D., Berdaliyeva F., Karan L., Nurmagambet S., Polukchi T., Pshenichnaya N., Sadyhova D.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of molecular diagnostic and epidemiology, Central Research Institute of Epidemiology, Novogireevskaya 3A, Moscow 111123, Russia, Arch Clin Infect Dis 17 (6), e129126 (2022)</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>Molecular identification of crimean-congo haemorrhagic fever virus in livestock ticks in the upper east region of ghana</t>
   </si>
   <si>
-    <t>Addo S., Agbodzi B., Ansah-owusu J., Asoala V., Baako B., Baidoo P., Bentil R., Diclaro J., Dunford J., Kumordjie S., Larbi J., Tawiah-mensah C., Wilson M., Yartey K., Yeboah C.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NAMRU-3, University of Ghana Noguchi Memorial Institute for Medical Research, P O Box LG 581, University of Ghana-Legon, Accra, Legon +233, Ghana, Unpublished</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>Collection and screening for cchfv of hyalomma marginatum questing unfed adults in thrace, turkey</t>
   </si>
   <si>
-    <t>Akyildiz G., Bircan R., Kar S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of Biology, Namik Kemal University, Degirmenalti Campus, Tekirdag, Suleymanpasa 59100, Turkey, Unpublished</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
     <t>Emerging viruses are an underestimated cause of undiagnosed febrile illness in uganda</t>
   </si>
   <si>
-    <t>Ashraf S., Balinandi S., Bugembe D., Bukenya H., Bwogi J., Byaruhanga T., Da silva filipe A., Davis C., Downing R., Jerome H., Kaleebu P., Kayiwa J., Kigozi B., Logan N., Lutwama J., Mcconnell W., Namuwulya P., Salazar M., Salazar-gonzalez J., Shepherd J., Sreenu V., Ssekagiri A., Ssemwanga D., Thomson E., Wilkie G., Willett B.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> MRC Centre for Virus Research, University of Glasgow, 464 Bearsden Road, Glasgow G61 1QH, United Kingdom, Unpublished</t>
   </si>
   <si>
@@ -290,9 +278,6 @@
     <t xml:space="preserve">The study titled "Emerging viruses are an underestimated cause of undiagnosed febrile illness in Uganda" by Ashraf S. et al. was published in the International Journal of Infectious Diseases. The article is available at: ([ijidonline.com](https://www.ijidonline.com/article/S1201-9712%2823%2900171-6/fulltext?utm_source=openai)) </t>
   </si>
   <si>
-    <t>Ashraf S., Burton C., Carmichael S., Filipe A., Love H., Richards K., Roddy S., Smollett K., Summers S., Thomson E., Tong L.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> MRC Centre for Virus Research, University of Glasgow, 464 Bearsden Road, Glasgow G61 1QH, United Kingdom,  MRC Centre for Virus Research, University of Glasgow, 464 Bearsden road, Glasgow G61 1QH, United Kingdom</t>
   </si>
   <si>
@@ -305,9 +290,6 @@
     <t>Human cases of cchfv in oman 2012-2014</t>
   </si>
   <si>
-    <t>Al-abaidani I., Al-abri S., Al-jardani A., Al-kindi H., Al-maani A., Al-mahrooqi S., Al-rawahi B., Almahrouqi S., Atkinson B., Bawakir S., Beeching N., Hewson R.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Research, Public Health England, Manor Farm Road, Salisbury, Wiltshire SP4 0JG, UK, Unpublished</t>
   </si>
   <si>
@@ -320,9 +302,6 @@
     <t>Crimean-congo hemorrhagic fever in uganda 2013-2019</t>
   </si>
   <si>
-    <t>Almberg M., Balinandi S., Klena J., Kyondo J., Lutwama J., Mugisha L., Mulei S., Nyakarahuka L., Shoemaker T., Tumusiime A., Whitmer S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> VSPB, CDC, 1600 Clifton Rd. NE, Atlanta, GA 30333, USA, Unpublished</t>
   </si>
   <si>
@@ -332,9 +311,6 @@
     <t>Whole genome sequencing of crimean-congo hemorrhagic fever orthonairovirus in iran</t>
   </si>
   <si>
-    <t>Azadmanesh K., Baniasadi V., Fazlalipour M., Fereydouni Z., Jalali T., Mohammadi T., Pouriayevali M., Qaedi H., Salehi-vaziri M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arboviruses and Viral Hemorrhagic Fevers Department (National Ref Lab), Pasteur Institute of Iran, No 69, Pasteur Ave, Tehran, Tehran 1316943551, Iran, Unpublished</t>
   </si>
   <si>
@@ -344,18 +320,12 @@
     <t>First whole genome isolation of crimean-congo haemorrhagic fever virus (cchfv) in tick species within ghana</t>
   </si>
   <si>
-    <t>Addo S., Agbodzi B., Ampadu R., Asoala V., Baako B., Behene E., Bentil R., Dadzie S., Diclaro J., Fox A., Harwood J., Kumordjie S., Letizia A., Mingle D., Mosore M., Nimo-paintsil S., Nyarko E., Oduro D., Tagoe J., Yeboah C.</t>
-  </si>
-  <si>
     <t>OQ441063, OQ441064, OQ441065</t>
   </si>
   <si>
     <t>Orthonairovirus haemorrhagiae in north macedonia, 2023</t>
   </si>
   <si>
-    <t>Bosevska G., Cadar D., Emmerich P., Osmani D., Toth E., Von possel R.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Virus Genomics and Evolution, Bernhard Nocht Institute for Tropical Medicine, Bernhard-Nocht-Strasse 74, Hamburg, Deutschland 20359, Deutschland, Unpublished</t>
   </si>
   <si>
@@ -368,9 +338,6 @@
     <t>Severe undifferentiated febrile illness outbreaks in the federal republic of sudan: a retrospective epidemiological &amp; diagnostic cohort study</t>
   </si>
   <si>
-    <t>Alzain M., Atkinson B., Bausch D., Beeching N., Bower H., Brooks T., Carter D., Dowall S., El halawi A., El karsany M., Eldegail M., Fletcher T., Furneaux J., Gannon B., Graham V., Hewson R., Mahmoud I., Mellors J., Mohamed R., Mohamednour S., Osborne J., Osman A., Pullan S., Semper A., Slack G., Taha R., Whitworth J.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Genomics of Rare and Emerging Human Pathogens, Public Health England, Manor Farm Road, Porton Down, Wiltshire SP4 0JG, United Kingdom, Unpublished</t>
   </si>
   <si>
@@ -380,9 +347,6 @@
     <t>Serological and virological evidence of crimean-congo haemorrhagic fever virus circulation in the human population of borno state, northeastern nigeria</t>
   </si>
   <si>
-    <t>Atkinson B., Baba S., Bell A., Bosworth A., Bukbuk D., Dowall S., Hewson R., Lewandowski K., Varghese A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Research and Technical Services, Public Health England, Manor Farm Road, Porton, Wiltshire SP4 0JG, UK, Unpublished</t>
   </si>
   <si>
@@ -395,9 +359,6 @@
     <t>Prevalence of crimean congo hemorrhagic fever virus (cchfv) in ixodid ticks in a hyper endemic region in turkey</t>
   </si>
   <si>
-    <t>Bursali A., Dundar E., Ekici M., Mutluay N., Ozkan M., Tekin S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Biology Department, Balikesir Universitey, Balikesir Universitesi FEF Biyoloji, Balikesir 10145, Turkiye, Unpublished</t>
   </si>
   <si>
@@ -407,9 +368,6 @@
     <t>GU324989, GU324990, GU324991, GU324992, GU324993, GU324994</t>
   </si>
   <si>
-    <t>Bordi L., Capobianchi M., Carletti F., Castilletti C., Chiappini R., Di caro A., Ippolito G., Lalle E.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Biorepository, National Institute for Infectious Diseases, Via Portuense 292, Rome, RM 00149, Italy,  Virology, Laboratory, Via Portuense 292, Rome 00149, Italy</t>
   </si>
   <si>
@@ -419,9 +377,6 @@
     <t>FJ445749, FJ472634</t>
   </si>
   <si>
-    <t>Bouzari S., Chinikar S., Jalali T., Mostafavi E., Shah-hosseini N., Shokrgozar M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arboviruses and Viral Haemorrhagic Fevers Laboratory (National Ref. Lab), Pasteur Institute of Iran, 69 Pasteur Ave, Tehran, Tehran 1316943551, Iran</t>
   </si>
   <si>
@@ -434,9 +389,6 @@
     <t>Tick-borne arbovirus and rickettsiae surveillance at livestock markets and slaughterhouses in western kenya: implications for dissemination and human infection</t>
   </si>
   <si>
-    <t>Bastos A., Chiuya T., Fevre E., Masiga D.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mbbu, ICIPE, ICIPE Road, Nairobi 00100, Kenya, Unpublished</t>
   </si>
   <si>
@@ -446,9 +398,6 @@
     <t>Identification and phylogenetic analysis of the latest isolated crimean-congohemorrhagic fever virus in xinjiang, china</t>
   </si>
   <si>
-    <t>Deng F., Guo R., Liu D., Liu J., Shen S., Shi J., Su Z., Wang Q., Yang J., Zhang Y.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Wuhan Institute of Virology, China Academy of Science, Xiaohongshan District No. 44, Wuhan, Hubei 430071, China, Unpublished</t>
   </si>
   <si>
@@ -458,9 +407,6 @@
     <t>Genetic diversity of crimean-congo hemorraghic fever virus in russia</t>
   </si>
   <si>
-    <t>Butenko A., Gmyl A., Gordeychuk I., Isaeva O., Klimentov A., Larichev V.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Chumakov Institute of Poliomyelitis and Viral Encephalitides, 27 km Kievskogo shosse, Moscow 142782, Russia, Unpublished</t>
   </si>
   <si>
@@ -470,9 +416,6 @@
     <t>Genetic characterization of the s and m segments of crimean congo hemorrhagic fever virus strains isolated in iran</t>
   </si>
   <si>
-    <t>Chinikar S., Li Q., Lundkvist K., Nilsson M., Nordstrom H., Plyusnin A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Centre for Microbiological Preparedness, Swedish Institute for Infectious Disease Control, Nobelsvag 18, Solna 171 82, Sweden, Unpublished</t>
   </si>
   <si>
@@ -494,9 +437,6 @@
     <t>Identification of diverse viruses in upper respiratory samples in dromedary camels from united arab emirates</t>
   </si>
   <si>
-    <t>Al hammadi Z., Al hosani F., Al muhairi S., Eltahir Y., Gerber S., Hall A., Khalafalla A., Li Y., Paden C., Queen K., Tao Y., Tong S., Yusof M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Division of Viral Diseases, Centers for Disease Control and Prevention, 1600 Clifton Rd, Atlanta, GA 30333, USA, Unpublished</t>
   </si>
   <si>
@@ -509,9 +449,6 @@
     <t>Detection of a non-fatal case of crimean-congo haemorrhagic fever imported into the uk (ex bulgaria), june 2014</t>
   </si>
   <si>
-    <t>Aarons E., Atkinson B., Brooks T., Dowall S., Glover S., Hewson R., Lumley S., Nijjar M., Petridou C., Simpson A., Staplehurst S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Research, Public Health England, Porton Down, Salisbury, Wilts SP40JG, UK, Unpublished</t>
   </si>
   <si>
@@ -524,9 +461,6 @@
     <t>Molecular phylogenetic study on s-segment of crimean-congo hemorrhagic fever (cchf) virus genome isolated from ticks in in west azerbaiajan and sistan and baluchestan provinces, iran, 2010</t>
   </si>
   <si>
-    <t>Ghalyanchi langrodi A., Langeroudi A., Majidzadeh K., Morovvati A., Razmyar J., Soleimani M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tasnim Biotechnology Research Center, AJA University of Medical Science, West Fatemi St, Tehran, Tehran 1411718541, Iran, Int. J. Infect. Dis. 16, E258 (2012)</t>
   </si>
   <si>
@@ -539,9 +473,6 @@
     <t>First detection of crimean-congo haemorrhagic fever virus in tick from migratory birds in italy</t>
   </si>
   <si>
-    <t>D'alessio S., Di domenico M., Di luca M., Goffredo M., Mancini G., Mancuso E., Marcacci M., Monaco F., Orsini M., Polci A., Spina F., Toma L.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Viral, Foreign Deseases of Animals, Istituto Zooprofilattico Sperimentale dell'Abruzzo e del Molise 'G. Caporale', Via Campo Boario, Teramo, Abruzzo 64100, Italy, Unpublished</t>
   </si>
   <si>
@@ -551,9 +482,6 @@
     <t>Genetic variation in the nucleoprotein gene of crimean-congo haemorrhagic fever virus</t>
   </si>
   <si>
-    <t>Berthet F., Marriott A., Nuttall P., Zeller H.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Marriott A.C., NERC Institute of Virology &amp; Environmental Microbiology, Mansfield Road, Oxford, OX1 3SR, United Kingdom, Unpublished</t>
   </si>
   <si>
@@ -566,9 +494,6 @@
     <t>Crimean congo hemorrhagic fever virus s segment sequence, strain matin</t>
   </si>
   <si>
-    <t>Hazlett L., Meissner J., Nichol S., Sato S., St. jeor S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Microbiology, University of Nevada, Reno, MS200/FA310, Reno, NV 89557, USA, Unpublished</t>
   </si>
   <si>
@@ -581,9 +506,6 @@
     <t>Cchf in ardabil</t>
   </si>
   <si>
-    <t>Habibzadeh S., Jeddi F., Mirzanejad-asl H., Mohammadi-ghalehbin B., Mohammadshahi J., Molaei S., Peeri doghaheh H., Soozangar N., Spotin A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Parasitolgy and Mycology, Tabriz University od Medical Sceinces, Golgasht Ave, Tabriz, Iran, Tabriz, East Azerbijan 5166/15731, Iran, Unpublished</t>
   </si>
   <si>
@@ -593,9 +515,6 @@
     <t>Detection of new crimean-congo hemorrhagic fever virus genotypes in ticks feeding on deer and wild boar, spain</t>
   </si>
   <si>
-    <t>Calero-bernal R., De la fuente J., Fernandez de mera I., Gortazar C., Habela M., Moraga fernandez A., Royo-hernandez L., Ruiz fons F.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Sanidad Animal, Instituto de Investigacion en Recursos Cinegeticos, Ronda de Toledo s/n, Ciudad Real 13071, Spain, Lancet (2019) In press</t>
   </si>
   <si>
@@ -608,9 +527,6 @@
     <t>Health risks associated with argasid ticks, transmitted pathogens and blood parasites in european griffon vulture (gyps fulvus) nestlings in spain</t>
   </si>
   <si>
-    <t>De la fuente J., Fernandez de mera I., Margalida A., Martinez J., Moraga-fernandez A., Munoz-hernandez C., Oliva-vidal P., Sanchez-sanchez M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of Science and Agroforestal Technology and Genetics, Institute for Game and Wildlife Research, Ronda Toledo 12, Ciudad Real, Ciudad Real 13005, Spain, Unpublished</t>
   </si>
   <si>
@@ -620,9 +536,6 @@
     <t>Survey of crimean-congo hemorrhagic fever enzootic focus, spain, 2011-2015</t>
   </si>
   <si>
-    <t>Calero-bernal R., Estrada-pena A., Habela M., Labiod N., Lasala F., Lopez P., Negredo A., Ramirez de arellano E., Sanchez-seco P., Sarria A., Tenorio A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arbovirus and Imported Viral Diseases, National Center of Microbiology, Institute of Health Carlos III, Ctra. Majadahonda-Pozuelo, km2, Majadahonda, Madrid 28220, Spain, Emerging Infect. Dis. 25 (6) (2019) In press</t>
   </si>
   <si>
@@ -632,9 +545,6 @@
     <t>Occurrence of the neglected arboviruses in the astrakhan region of russia for 2018 season: the development of multiplex pcr assays and analysis of mosquitoes, ticks, and human blood sera</t>
   </si>
   <si>
-    <t>Akishkin V., Arjba T., Azarian A., Babaeva M., Bashkina O., Butenko A., Gintsburg A., Gushchin V., Kozlova A., Kuznetsova N., Larichev V., Nikeshina N., Nikiforova M., Rubalsky O., Shchetinin A., Tkachuk A., Vakalova E.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Pathogenic Microorganisms Variability Lab, N.F. Gamaleya Research Center of Epidemiology and Microbiology, Gamaleya str., 16, Moscow 123098, Russia, Unpublished</t>
   </si>
   <si>
@@ -647,9 +557,6 @@
     <t>Outcome of the entomological monitoring for the crimean-congo haemorrhagic fever virus in the western and southern regions of kazakhstan in 2021-2022</t>
   </si>
   <si>
-    <t>Nurmakhanov T., Sadovskaya V., Shevtsov A., Tokmurziyeva G., Tukhanova N., Turebekov N.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Laboratory of applied genetics, National center for biotechnology, Kazakhstan, Kurgalzhynskoye road, 13/5, Astana, Akmola Region 010000, Kazakhstan, Unpublished</t>
   </si>
   <si>
@@ -659,9 +566,6 @@
     <t>Transmission dynamics of crimean congo haemorrhagic fever virus (cchfv); evidence of circulation in humans, livestock, and rodents in diverse ecologies in kenya</t>
   </si>
   <si>
-    <t>Junglen S., Kopp A., Ogola E., Omoga D., Osalla J., Sang R., Slothouwer I., Tchouassi D., Torto B., Venter M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Human Health, ICIPE, ICIPE Road, off Kasarani Road, Nairobi 00100, Kenya, Unpublished</t>
   </si>
   <si>
@@ -671,9 +575,6 @@
     <t>Genetic analysis of s gene of cchfv in humans in turkey</t>
   </si>
   <si>
-    <t>Aydin K., Koksal I., Ozdarendeli A., Tonbak S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Virology, Firat University, Firat, Elazig 23119, Turkey, Unpublished</t>
   </si>
   <si>
@@ -695,9 +596,6 @@
     <t>LT673890</t>
   </si>
   <si>
-    <t>Glass P., Jennings G., Lofts R., Miller M., Parker M., Schoepp R., Smith J., Spik K.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Michael D. Parker, Virology Divison, USAMRIID, Bldg. 1425 Fort Detrick, Frederick, MD 21702, USA</t>
   </si>
   <si>
@@ -710,9 +608,6 @@
     <t>Cchf virus, isolated from ticks in tajikistan</t>
   </si>
   <si>
-    <t>Chausov E., Kononova Y., Petrova I., Shestopalov A., Tishkova F.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Microscopic Researches, State Research Center of Virology and Biotechnology 'Vector', Koltsovo, Novosibirsk Region 630559, Russia, Unpublished</t>
   </si>
   <si>
@@ -725,9 +620,6 @@
     <t>Molecular epidemiology and diagnostics of crimean-congo hemorrhagic fever in southern russia</t>
   </si>
   <si>
-    <t>Antonov V., Govorukhina M., Karan L., Krasnova E., Maleev V., Obukhov I., Platonov A., Shipulin G., Shvager M., Yazyshina S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Central Research Institute of Epidemiology, Novogireevskaya Str. 3A, Moscow 111123, Russia, Unpublished</t>
   </si>
   <si>
@@ -740,9 +632,6 @@
     <t>Sequencing and analysis of s gene of cchfv</t>
   </si>
   <si>
-    <t>Bouloy M., Feng C., Prehaud C., Tang Q.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prehaud C.J., Laboratoire des Bunyavirides, Institut Pasteur, 25 rue du Dr Roux, 75724 Paris Cedex 15, FRANCE, Zhonghua Wei Sheng Wu Xue He Mian Yi Xue Za Zhi 19, 461-465 (1999)</t>
   </si>
   <si>
@@ -755,9 +644,6 @@
     <t>Full genome sequencing and phylogenetic characterization of crimean congo hemorrhagic fever virus in spain</t>
   </si>
   <si>
-    <t>Arsuaga M., Fernandez cruz A., Goyanes M., Hernandez L., Negredo A., Perez sautu U., Ramirez de arellano E., Sanchez-seco M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arbovirus and Imported Viral Diseases Laboratory, National Center of Microbiology, Institute of Health Carlos III, Crta. Majadahonda a Pozuelo Km 2, Madrid 28220, Spain, Unpublished</t>
   </si>
   <si>
@@ -767,9 +653,6 @@
     <t>Assessment of humoral and cellular immune responses elicited by a dna based vaccine targeting crimean congo hemorrhagic fever virus glycoprotein gc in immunocompetent balb/c mouse model</t>
   </si>
   <si>
-    <t>Coleri cihan A., Farzani T., Ozkul A., Sahin E.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Biology, Ankara University, Dogol Street Tandogan, Ankara 06100, Turkey, Unpublished</t>
   </si>
   <si>
@@ -779,9 +662,6 @@
     <t>Molecular studies of cchf virus circulating in north india</t>
   </si>
   <si>
-    <t>Chhabra M., Singh P., Venkatesh S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Biotechnology division, National Centre for Diseases Control, 22-Sham Nath Marg, Delhi, Delhi 110054, India, Unpublished</t>
   </si>
   <si>
@@ -794,18 +674,12 @@
     <t>Novel segmented rna jingmenvirus group isolated from human</t>
   </si>
   <si>
-    <t>Agafonov A., Gladysheva A., Kotenev E., Loktev V., Sementsova A., Ternovoi V., Volynkina A., Zaykovskaya A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of Molecular Virology, State Research Center of Virology and Biotehnology 'Vector', Koltsovo, Russia 630559, Russia, Unpublished</t>
   </si>
   <si>
     <t>MN218693, MN218694, MN218695, MN218696</t>
   </si>
   <si>
-    <t>Kolosov A., Kotenev E., Volynkina A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Laboratory on Natural Focal Infections, Stavropol State Research Anti-Plague Institute, Sovetskaya str. 13-15, Stavropol, Stavropol Region 355035, Russian Federation,  Laboratory on Natural Focal Infections, Stavropol State Research Anti-Plague Institute, Sovetskaya str. 13-15, Stavropol, Stavropol region 355017, Russian Federation</t>
   </si>
   <si>
@@ -815,9 +689,6 @@
     <t>Phylogenetic characterisation of crimean-congo hemorrhagic fever virus detected in african blue ticks feeding on cattle in a ugandan abattoir</t>
   </si>
   <si>
-    <t>Allen D., Frost S., Hewson R., Stubbs S., Waiswa P., Wampande E.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Infectious Disease Epidemiology, London School of Hygiene and Tropical Medicine, Keppel Street, London WC1E 7HT, UK, Preprints (Basel) (2021) In press</t>
   </si>
   <si>
@@ -827,9 +698,6 @@
     <t>The characterization of crimean-congo haemorrhagic fever virus glycoproteins, The crimean-congo haemorrhagic fever virus genetic analysis</t>
   </si>
   <si>
-    <t>Deng F., Hu Z., Li T., Meng W., Sun S., Wang H., Xia Y., Zhang Y., Zhou Z.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Molecular Virology Lab, Wuhan Institution of Virology, CAS, No. 44, Xiaohongshan Middle District, Wuchan District, Wuhan, Hubei 430071, China, Unpublished</t>
   </si>
   <si>
@@ -839,9 +707,6 @@
     <t>A focal outbreak of crimean congo hemorrhagic fever in ahmadabad, india, 2011</t>
   </si>
   <si>
-    <t>Mourya D., Yadav P.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> VR-HCL, National Institute of Virology, Microbial Containment Complex, Sus Road, Pashan, Pune, Maharashtra 411021, India, Unpublished</t>
   </si>
   <si>
@@ -854,9 +719,6 @@
     <t>The characterization of cchfv glycoproteins, The crimean-congo haemorrhagic fever virus genetics and analysis</t>
   </si>
   <si>
-    <t>Deng F., Hu Z., Li T., Meng W., Sun S., Wang H., Zhang Y., Zhou Z.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Molecular Virology and Bioengeneering Research Group, Wuhan Institution of Virology, CAS, Xiaohongshan 44#, Wuhan, Hubei 430071, China, J. Gen. Virol. (2010) In press</t>
   </si>
   <si>
@@ -866,9 +728,6 @@
     <t>GU477492, GU477493, GU477494</t>
   </si>
   <si>
-    <t>Abdulall A., Bendary H., Rasslan F., Zaki A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Microbiology and Immunology, Faculty of Pharmacy (Girls), Al-Azhar University, Dr Abd El-Shennawy, Nasr City, Cairo 11765, Egypt,  Microbiology and Immunology, Faculty of Pharmacy (Girls), Al-Azhar University, Dr Abd El-Shennawy, Nasr city, Cairo 11765, Egypt</t>
   </si>
   <si>
@@ -881,9 +740,6 @@
     <t>Complete genome sequencing of crimean-congo haemorrhagic fever virus (cchfv) directly from clinical samples: a comparative study between targeted enrichment and metagenomic approaches, Recovery of complete genome sequences of crimean-congo haemorrhagic fever virus (cchfv) directly from clinical samples: a comparative study between targeted enrichment and metagenomic approaches, Recovery of complete genome sequences of crimean-congo haemorrhagic fever virus through targeted next-generation sequencing approaches: a comparative study between multiplex tiling pcr and probe hybridization capture</t>
   </si>
   <si>
-    <t>Afrough B., Allen D., D'addiego J., Elaldi N., Fletcher T., Hewson R., Kurosaki Y., Leblebicioglu H., Shah S., Wand N.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Research &amp; Evaluation, UK Health Security Agency, Manor Farm Road, Salisbury, Wiltshire SP4 0JG, United Kingdom, Unpublished</t>
   </si>
   <si>
@@ -893,9 +749,6 @@
     <t>OQ454691, OQ454692, OQ454693, OQ454694, OQ454695, OQ454696, OQ454697, OQ454698, OQ454699, OQ454700, OQ454701, OQ454702, OQ454703, OQ454704, OQ454705, OQ454706, OQ454707, OQ454708, OQ454709, OQ454710, OQ454711, OQ454712, OQ454713, OQ454714, OQ454715, OQ454716, OQ454717, OQ454718, OQ454719, OQ454720, OQ454721, OQ454722, OQ454723, OQ454724, OQ454725, OQ454726, OQ454727, OQ454728, OQ454729, OQ454730, OQ454731, OQ454732, OQ454733, OQ454734, OQ454735, OQ454736, OQ454737, OQ454738, OQ454739, OQ454740, OQ454741, OQ454742, OQ454743, OQ454744, OQ454745, OQ454746, OQ454747, OQ454748, OQ454749, OQ454750, OQ454777, OQ454778, OQ454779, OQ454780, OQ454781, OQ454782, OQ454783, OQ454784, OQ454785, OQ454786, OQ454787, OQ454788, OQ454789, OQ454790, OQ454791, OQ454792, OQ454793, OQ454794, OQ454795, OQ454796, OQ454797, OQ454798, OQ454799, OQ454800, OQ454801, OQ454802, OQ454803, OQ454804, OQ454805, OQ454806, OQ454807, OQ454808, OQ454809, OQ454810, OQ454811, OQ454812, OQ454813, OQ454814, OQ454815, OQ454816, OQ454817, OQ454818, OQ454819, OQ454820, OQ454821, OQ454822, OQ454823, OQ454824, OQ454825, OQ454826, OQ454827, OQ454828, OQ454829, OQ454830, OQ454831, OQ454832, OQ454833, OQ454834, OQ454835, OQ454836, OQ866631, OQ866632, OQ866633, PP735307, PP735308, PP735309, PP735310, PP735311, PP735312, PP735313, PP735314, PP735315, PP735316, PP735317, PP735318, PP735319, PP735320, PP735321, PP735322, PP735323, PP735324, PP735325, PP735326, PP735327, PP735328, PP735329, PP735330, PP735331, PP735332, PP735333, PP735334, PP735335, PP735336, PP735337, PP735338, PP735339, PP735340, PP735341, PP735342, PP735343, PP735344, PP735345, PP735346, PP735347, PP735348, PP735349, PP735350, PP735351, PP735352, PP735353, PP735354, PP735355, PP735356, PP735357, PP735358, PP735359, PP735360, PP735361, PP735362, PP735363, PP735364, PP735365, PP735366, PP735367, PP735368, PP735369, PP735370, PP735371, PP735372, PP735373, PP735374, PP735375</t>
   </si>
   <si>
-    <t>Dai X., Feng C., Hang C., Meng W., Sun S., Wang X., Zhang Y.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> The Center for Disease Control and Prevention of Xinjiang Uygur Autonomous Region, Xinjiang Key Lab of Biological Resources and Genetic Engineering, College of Life Science and Technology, Xinjiang University, Urumuqi 830046, P.R. China</t>
   </si>
   <si>
@@ -905,9 +758,6 @@
     <t>Detection of autochthonic virus strain responsible for outbreak of crimean-congo haemorrhagic fever in north macedonia, july to august 2023, Increased clinical vigilance identified additional human cases and genetically diverse isolates of crimean-congo haemorrhagic fever virus in north macedonia</t>
   </si>
   <si>
-    <t>Abraham A., Banovic P., Banyai K., Bogdan I., Cana F., Christova I., Cvetanovska M., Cvetkovikj A., Djadjovski I., Gorfol T., Grozdanovski K., Jakimovski D., Kemenesi G., Kostoulas P., Kuczmog A., Lanszki Z., Meletis E., Mijatovic D., Rangelov G., Simin V., Spasovska K., Tauber Z., Urban P., Zana B.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Szentagothai Research Center, University of Pecs, Ifjusag Utja 20, Pecs, Baranya 7624, Hungary,  Szentagothai Research Center, University of Pecs, Ifjusag utja 20, Pecs, Baranya 7624, Hungary, Unpublished</t>
   </si>
   <si>
@@ -917,18 +767,12 @@
     <t>Molecular epidemiology and phylogeny of crimean-congo haemorrhagic fever (cchf) virus of ixodid ticks in khorasan-e-razavi province of iran, Molecular epidemiology and phylogeny of crimean-congo hemorrhagic fever (cchf) virus of ixodid ticks in khorasan-e-razavi province of iran</t>
   </si>
   <si>
-    <t>Chinikar S., Maghsood H., Nabian S., Shayan P.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Parasitology, Faculty of Veterinary Medicine, University of Tehran, Enghalab Square, Tehran 009821, Iran,  Parasitology, Faculty of Veterinary Medicine, University of Tehran, Enghalab Square, Tehran, Tehran 009821, Iran, Unpublished</t>
   </si>
   <si>
     <t>KP682503, KP742979</t>
   </si>
   <si>
-    <t>Aktas M., Altas K., Ergin S., Gargili A., Midilli K., Ozturk R., Sengoz G., Vatansever Z., Yilmaz G.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Microbiology and Clinical Microbiology, Cerrahpasa Medical Faculty of Istanbul University, Temel Bilimler Binasi, Fatih - Istanbul 34303, Turkey,  Microbiology and Clinical Microbiology, Cerrahpasa Medical Fakulty of Istanbul University, Temel Bilimler Binasi, Fatih - Istanbul 34303, Turkey</t>
   </si>
   <si>
@@ -941,18 +785,12 @@
     <t>Deposition of the nucleotide sequence of s, m, and l segments of cchf virus isolates derived from human blood serum of the patient in the south kazakhstan region, Deposition of the nucleotide sequences of s, m, and l segments of cchf virus obtained by sequencing of samples from ticks of the south kazakhstan region</t>
   </si>
   <si>
-    <t>Atkinson B., Atshabar B., Berezin V., Deryabin P., Hewson R., Nurmakhanov T., Sansyzbaev Y., Shevtsov A., Vilkova A., Yeskhojayev O.</t>
-  </si>
-  <si>
     <t>KX096700, KX096701, KX096702, KX096703, KX096704, KX096705, KX096706, KX129730, KX129731, KX129732, KX129733, KX129734, KX129735, KX129736, KX129737, KX129738, KX129739, KX458183</t>
   </si>
   <si>
     <t>An iran-kerman22 related strain of crimean-congo hemorrhagic fever orthonairovirus, Crimean-ongo haemorrhagic fever among healthcare workers in iran 2000-2018, a report of national reference laboratory</t>
   </si>
   <si>
-    <t>Azad-manjiri S., Azadmanjiri S., Azizizadeh S., Baniasadi V., Fazlalipour M., Fereydouni Z., Ghalejoogh M., Hosseini M., Jalai T., Jalali T., Khakifirouz S., Mohammadi T., Pouriayevali M., Salehi-vaziri M., Tavakoli M., Tavakolirad M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arboviruses and Viral Hemorrhagic Fevers Department (National Ref. Lab), Pasteur Institute of Iran, No. 69, Pasteur Ave., Tehran 1316943551, Iran,  Arboviruses and Viral Hemorrhagic Fevers Department (National Ref. Lab.), Pasteur Institute of Iran, No. 69, Pasteur Ave., Tehran 1316943551, Iran, Unpublished</t>
   </si>
   <si>
@@ -962,9 +800,6 @@
     <t>An isolate of cchf virus from an iranian fulminant cchf patient, An isolate of cchf virus from an iranian patient in north of iran, Crimean congo hemorrhagic fever in qeshm island, iran, eid al adha (eid qorban) 2017</t>
   </si>
   <si>
-    <t>Azad-manjiri S., Azizizadeh S., Baniasadi V., Fazlalipour M., Fereydouni Z., Ghasemian R., Hosseini M., Jalali T., Jamshidi Y., Khakifirouz S., Mirahmadi R., Mirghiasi M., Mohammadi T., Pouriayevali M., Salehi-vaziri M., Tavakolirad M., Zarandi R.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Virology, Tehran University of Medical Sciences, No 69, Pasteur Ave, Tehran 0098, Iran,  Virology, Tehran University of Medical Sciences, No. 69 Pasteur Ave., Tehran 0098, Iran,  Virology, Tehran University of Medical Sciences, No. 69, Pasteur Ave., Tehran 0098, Iran, Unpublished</t>
   </si>
   <si>
@@ -974,9 +809,6 @@
     <t>KT899991, KY274404, MG456911</t>
   </si>
   <si>
-    <t>Ajati A., Azati A., Dai X., Feng C., Hang C., Ma J., Meng W., Sun S., Wang X., Xie Y., Zhang F., Zhang Y., Zhu H.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> College of Life Science and Technology, Xinjiang University, 14 Shengli Road, Urumqi, Xinjiang 830046, China,  Xinjiang Center for Disease Control and Prevention, College of Life Science and Technology, Xinjiang University, Urumqi, Xinjiang 830002, China</t>
   </si>
   <si>
@@ -989,9 +821,6 @@
     <t>Cchf genetic variety research</t>
   </si>
   <si>
-    <t>Gao D., Han L., Tang Q., Tao X., Zhao X.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Institute of Epidemiology and Microbiology, Chinese Academy of Preventive Medicine (CAPM), P. O. Box 5 Changping, Beijing 102206, China,  Institute of Epidemiology and Microbiology, Chinese Academy of Preventive Medicine (CAPM), P.O. Box 5 Changping, Beijing 102206, China,  Institute of Epidemiology and Microbiology, Chinese Academy of Preventive Medicine, P. O. Box 5 Changping, Beijing 102206, P.R. China, Unpublished</t>
   </si>
   <si>
@@ -1001,9 +830,6 @@
     <t>Molecular characterization of s and m segments of crimean congo hemorrhagic fever virus in turkey</t>
   </si>
   <si>
-    <t>Aydin H., Timurkan M.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of Virology, Ataturk University, Faculty of Veterinary Medicine, Erzurum 25240, Turkey,  Departmet of Virology, Ataturk University, Faculty of Veterinary Medicine, Erzurum 25240, Turkey, Unpublished</t>
   </si>
   <si>
@@ -1013,9 +839,6 @@
     <t>Crimean-congo virus in stavropol region of russia, 2011, Genetic monitoring of crimean-congo hemorrhagic fever virus in the south of the european part of russia</t>
   </si>
   <si>
-    <t>Kulichenko A., Malyshev B., Volynkina A., Yashina L.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Laboratory of Virology, Stavropol Research Anti-Plague Institute, Sovjetskaya St., 13-15, Stavropol, Stavropol Region 355000, Russian Federation,  PCR Diagnostics, State Research Center of Virology and Biotechnology 'Vector', SRC VB Vector, Koltsovo, Novosibirsk region 630559, Russia, Probl Osobo Opas Infekc 4 (114), 80-85 (2012), Unpublished</t>
   </si>
   <si>
@@ -1028,9 +851,6 @@
     <t>Epidemiological analysis of crimean-congo hemorrhagic fever infection case on the territory of crimean federal district in 2015 caused by a new genetic variants of the virus</t>
   </si>
   <si>
-    <t>Burlachenko A., Kotenev E., Kulichenko A., Lisitskaya Y., Pisarenko S., Popova A., Shaposhnikova L., Volynkina A.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Laboratory of Natural-Focal Infections, Stavropol State Research Anti-Plague Institute, Sovetskaya Str. 13-15, Stavropol, Stavropol Region 355017, Russian Federation,  Laboratory of Natural-Focal Infections, Stavropol State Research Anti-Plague Institute, Sovetskaya str. 13-15, Stavropol, Stavropol region 355017, Russian Federation, Zh. Mikrobiol. Epidemiol. Immunobiol. (2016) In press</t>
   </si>
   <si>
@@ -1043,9 +863,6 @@
     <t>The current status of tick populations in istanbul and their biorisks in terms of cchf and public health</t>
   </si>
   <si>
-    <t>Akyildiz G., Gargili keles A., Zarrabi ahrabi S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Faculty of Health Sciences/Basic Health Sciences Department, Marmara University, M.U. Basibuyuk Campus, 9/4/1, Maltepe, Istanbul 34854, Turkey, Unpublished</t>
   </si>
   <si>
@@ -1055,9 +872,6 @@
     <t>Partial sequence of cchf virus l segment</t>
   </si>
   <si>
-    <t>Meissner J., Nichol S., St. jeor S.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Microbiology, University of Nevada, Reno, 1664 North Virginia Street, Reno, NV 89557, USA, Unpublished</t>
   </si>
   <si>
@@ -1065,9 +879,6 @@
   </si>
   <si>
     <t>AY422208, AY422209</t>
-  </si>
-  <si>
-    <t>Ali Q., Ammar M., Ansari S., Haider S., Hakim R., Ikram A., Jamal Z., Rehman Z., Salman M., Umair M.</t>
   </si>
   <si>
     <t xml:space="preserve"> Department of Virology, National Institute of Health, Park Road, Chak Shahzad, Islamabad, Islamabad 44000, Pakistan</t>
@@ -1476,6 +1287,195 @@
   </si>
   <si>
     <t>32655079, 26902209</t>
+  </si>
+  <si>
+    <t>Tang Q., Gao D., Han L., Zhao X., Tao X.</t>
+  </si>
+  <si>
+    <t>Platonov A., Karan L., Shipulin G., Maleev V., Yazyshina S., Antonov V., Krasnova E., Govorukhina M., Karan L., Shipulin G., Yazyshina S., Shvager M., Obukhov I.</t>
+  </si>
+  <si>
+    <t>Meissner J., Sato S., Hazlett L., St. jeor S., Nichol S.</t>
+  </si>
+  <si>
+    <t>Prehaud C., Tang Q., Bouloy M., Feng C.</t>
+  </si>
+  <si>
+    <t>Meissner J., St. jeor S., Nichol S.</t>
+  </si>
+  <si>
+    <t>Sun S., Zhang Y., Dai X., Ma J., Zhang F., Meng W., Wang X., Feng C., Hang C., Zhu H., Azati A., Meng W., Wang X., Ajati A., Dai X., Ma J., Zhang F., Zhu H., Feng C., Hang C., Meng W., Wang X., Ajati A., Dai X., Ma J., Zhang F., Zhu H., Feng C., Hang C., Xie Y.</t>
+  </si>
+  <si>
+    <t>Li Q., Nordstrom H., Chinikar S., Plyusnin A., Lundkvist K., Nilsson M.</t>
+  </si>
+  <si>
+    <t>Midilli K., Gargili A., Ergin S., Sengoz G., Gargili A., Vatansever Z., Ergin S., Aktas M., Yilmaz G., Gargili A., Yilmaz G., Sengoz G., Ozturk R., Altas K.</t>
+  </si>
+  <si>
+    <t>Ozdarendeli A., Aydin K., Tonbak S., Koksal I.</t>
+  </si>
+  <si>
+    <t>Feng C., Zhang Y., Sun S., Meng W., Dai X., Sun S., Meng W., Dai X., Sun S., Dai X., Meng W., Hang C., Wang X.</t>
+  </si>
+  <si>
+    <t>Carletti F., Di caro A., Capobianchi M., Castilletti C., Bordi L., Lalle E., Castilletti C., Capobianchi M., Ippolito G., Bordi L., Lalle E., Chiappini R.</t>
+  </si>
+  <si>
+    <t>Xia Y., Zhou Z., Meng W., Hu Z., Wang H., Zhang Y., Sun S., Li T., Hu Z., Wang H., Deng F.</t>
+  </si>
+  <si>
+    <t>Bursali A., Tekin S., Mutluay N., Ekici M., Ozkan M., Dundar E.</t>
+  </si>
+  <si>
+    <t>Zhou Z., Meng W., Deng F., Wang H., Li T., Zhang Y., Sun S., Hu Z.</t>
+  </si>
+  <si>
+    <t>Majidzadeh K., Soleimani M., Ghalyanchi langrodi A., Morovvati A., Soleimani M., Morovvati A., Razmyar J., Langeroudi A.</t>
+  </si>
+  <si>
+    <t>Yadav P., Mourya D.</t>
+  </si>
+  <si>
+    <t>Petrova I., Kononova Y., Chausov E., Shestopalov A., Tishkova F.</t>
+  </si>
+  <si>
+    <t>Volynkina A., Yashina L., Kulichenko A., Malyshev B., Volynkina A.</t>
+  </si>
+  <si>
+    <t>Chinikar S., Shah-hosseini N., Bouzari S., Jalali T., Shokrgozar M., Mostafavi E.</t>
+  </si>
+  <si>
+    <t>Lumley S., Atkinson B., Dowall S., Simpson A., Aarons E., Petridou C., Nijjar M., Glover S., Brooks T., Atkinson B., Hewson R., Staplehurst S.</t>
+  </si>
+  <si>
+    <t>Maghsood H., Nabian S., Chinikar S., Shayan P.</t>
+  </si>
+  <si>
+    <t>Popova A., Volynkina A., Kulichenko A., Lisitskaya Y., Burlachenko A., Lisitskaya Y., Shaposhnikova L., Kotenev E., Pisarenko S.</t>
+  </si>
+  <si>
+    <t>Baniasadi V., Fazlalipour M., Salehi-vaziri M., Ghasemian R., Jalali T., Jamshidi Y., Mohammadi T., Azad-manjiri S., Hosseini M., Azizizadeh S., Mirahmadi R., Khakifirouz S., Pouriayevali M., Jalali T., Mohammadi T., Fereydouni Z., Azad-manjiri S., Hosseini M., Tavakolirad M., Azizizadeh S., Khakifirouz S., Mirghiasi M., Jalali T., Khakifirouz S., Azad-manjiri S., Zarandi R., Salehi-vaziri M., Fazlalipour M.</t>
+  </si>
+  <si>
+    <t>Singh P., Chhabra M., Venkatesh S.</t>
+  </si>
+  <si>
+    <t>Klimentov A., Butenko A., Larichev V., Isaeva O., Gordeychuk I., Gmyl A.</t>
+  </si>
+  <si>
+    <t>Deryabin P., Nurmakhanov T., Atshabar B., Sansyzbaev Y., Berezin V., Yeskhojayev O., Vilkova A., Shevtsov A., Hewson R., Sansyzbaev Y., Atshabar B., Yeskhojayev O., Vilkova A., Shevtsov A., Hewson R., Atkinson B.</t>
+  </si>
+  <si>
+    <t>Bukbuk D., Dowall S., Lewandowski K., Bosworth A., Baba S., Varghese A., Bell A., Atkinson B., Hewson R.</t>
+  </si>
+  <si>
+    <t>Guo R., Shen S., Zhang Y., Shi J., Su Z., Liu D., Liu J., Yang J., Wang Q., Zhang Y., Deng F.</t>
+  </si>
+  <si>
+    <t>Ramirez de arellano E., Hernandez L., Goyanes M., Arsuaga M., Fernandez cruz A., Negredo A., Sanchez-seco M., Perez sautu U.</t>
+  </si>
+  <si>
+    <t>Li Y., Khalafalla A., Paden C., Yusof M., Eltahir Y., Al hammadi Z., Tao Y., Queen K., Al hosani F., Gerber S., Hall A., Al muhairi S., Paden C., Tao Y., Khalafalla A., Yusof M., Eltahir Y., Al hammadi Z., Queen K., Al hosani F., Gerber S., Hall A., Al muhairi S., Tong S.</t>
+  </si>
+  <si>
+    <t>Sahin E., Farzani T., Coleri cihan A., Ozkul A.</t>
+  </si>
+  <si>
+    <t>Atkinson B., Al-abri S., Al-kindi H., Bawakir S., Al-jardani A., Al-abaidani I., Al-mahrooqi S., Al-maani A., Almahrouqi S., Al-rawahi B., Beeching N., Hewson R.</t>
+  </si>
+  <si>
+    <t>Negredo A., Habela M., Ramirez de arellano E., Lasala F., Lopez P., Sarria A., Labiod N., Calero-bernal R., Tenorio A., Estrada-pena A., Sanchez-seco P.</t>
+  </si>
+  <si>
+    <t>Baniasadi V., Qaedi H., Jalali T., Pouriayevali M., Fazlalipour M., Mohammadi T., Fereydouni Z., Azadmanesh K., Salehi-vaziri M.</t>
+  </si>
+  <si>
+    <t>Jalai T., Pouriayevali M., Mohammadi T., Fereydouni Z., Tavakolirad M., Khakifirouz S., Azadmanjiri S., Hosseini M., Ghalejoogh M., Azizizadeh S., Baniasadi V., Fazlalipour M., Jalali T., Mohammadi T., Fereydouni Z., Tavakoli M., Azad-manjiri S., Hosseini M., Ghalejoogh M., Khakifirouz S., Azizizadeh S., Baniasadi V., Fazlalipour M., Salehi-vaziri M.</t>
+  </si>
+  <si>
+    <t>Mancuso E., Polci A., D'alessio S., Toma L., Di luca M., Orsini M., Di domenico M., Marcacci M., Mancini G., Spina F., Goffredo M., Monaco F.</t>
+  </si>
+  <si>
+    <t>Moraga fernandez A., Royo-hernandez L., Habela M., Ruiz fons F., Calero-bernal R., Gortazar C., De la fuente J., Fernandez de mera I.</t>
+  </si>
+  <si>
+    <t>Bower H., Carter D., El karsany M., Alzain M., Gannon B., Mohamed R., Mahmoud I., Eldegail M., Taha R., El halawi A., Osman A., Mohamednour S., Semper A., Atkinson B., Dowall S., Furneaux J., Graham V., Mellors J., Osborne J., Slack G., Brooks T., Hewson R., Beeching N., Whitworth J., Bausch D., Gannon B., Fletcher T., Pullan S.</t>
+  </si>
+  <si>
+    <t>Volynkina A., Kotenev E., Kolosov A.</t>
+  </si>
+  <si>
+    <t>Ternovoi V., Gladysheva A., Sementsova A., Zaykovskaya A., Volynkina A., Kotenev E., Agafonov A., Loktev V.</t>
+  </si>
+  <si>
+    <t>Chiuya T., Masiga D., Bastos A., Fevre E.</t>
+  </si>
+  <si>
+    <t>Akyildiz G., Kar S., Bircan R.</t>
+  </si>
+  <si>
+    <t>Nikiforova M., Shchetinin A., Kuznetsova N., Butenko A., Kozlova A., Larichev V., Vakalova E., Babaeva M., Arjba T., Akishkin V., Azarian A., Nikeshina N., Rubalsky O., Bashkina O., Tkachuk A., Gintsburg A., Kozlova A., Butenko A., Gushchin V.</t>
+  </si>
+  <si>
+    <t>Timurkan M., Aydin H.</t>
+  </si>
+  <si>
+    <t>Bendary H., Rasslan F., Zaki A., Zaki A., Abdulall A.</t>
+  </si>
+  <si>
+    <t>Wampande E., Allen D., Frost S., Waiswa P., Allen D., Hewson R., Frost S., Stubbs S.</t>
+  </si>
+  <si>
+    <t>Balinandi S., Whitmer S., Nyakarahuka L., Tumusiime A., Kyondo J., Mugisha L., Almberg M., Lutwama J., Shoemaker T., Klena J., Mulei S.</t>
+  </si>
+  <si>
+    <t>Umair M., Haider S., Jamal Z., Ammar M., Hakim R., Ali Q., Hakim R., Jamal Z., Jamal Z., Ammar M., Haider S., Ali Q., Hakim R., Jamal Z., Haider S., Ammar M., Ali Q., Hakim R., Rehman Z., Ikram A., Haider S., Ammar M., Ali Q., Hakim R., Salman M., Ansari S.</t>
+  </si>
+  <si>
+    <t>Ashraf S., Love H., Burton C., Carmichael S., Filipe A., Roddy S., Smollett K., Summers S., Tong L., Richards K., Thomson E.</t>
+  </si>
+  <si>
+    <t>Zarrabi ahrabi S., Akyildiz G., Gargili keles A.</t>
+  </si>
+  <si>
+    <t>Moraga-fernandez A., Sanchez-sanchez M., Munoz-hernandez C., Oliva-vidal P., Martinez J., Margalida A., De la fuente J., Fernandez de mera I.</t>
+  </si>
+  <si>
+    <t>Ashraf S., Jerome H., Bugembe D., Ssemwanga D., Byaruhanga T., Kayiwa J., Downing R., Salazar-gonzalez J., Salazar M., Shepherd J., Davis C., Logan N., Sreenu V., Wilkie G., Da silva filipe A., Ssekagiri A., Namuwulya P., Bukenya H., Kigozi B., Mcconnell W., Willett B., Balinandi S., Lutwama J., Kaleebu P., Bwogi J., Thomson E.</t>
+  </si>
+  <si>
+    <t>Abuova G., Pshenichnaya N., Karan L., Berdaliyeva F., Aliyev D., Sadyhova D., Polukchi T., Nurmagambet S.</t>
+  </si>
+  <si>
+    <t>Omoga D., Tchouassi D., Venter M., Ogola E., Osalla J., Kopp A., Slothouwer I., Torto B., Junglen S., Sang R.</t>
+  </si>
+  <si>
+    <t>Addo S., Bentil R., Baako B., Yartey K., Ansah-owusu J., Tawiah-mensah C., Agbodzi B., Kumordjie S., Yeboah C., Asoala V., Dunford J., Larbi J., Baidoo P., Wilson M., Diclaro J.</t>
+  </si>
+  <si>
+    <t>Bentil R., Addo S., Mosore M., Kumordjie S., Yeboah C., Agbodzi B., Behene E., Tagoe J., Baako B., Asoala V., Ampadu R., Mingle D., Nyarko E., Fox A., Letizia A., Diclaro J., Oduro D., Nimo-paintsil S., Harwood J., Dadzie S.</t>
+  </si>
+  <si>
+    <t>D'addiego J., Shah S., Elaldi N., Allen D., Wand N., Afrough B., Fletcher T., Kurosaki Y., Leblebicioglu H., Wand N., Hewson R.</t>
+  </si>
+  <si>
+    <t>Mohammadi-ghalehbin B., Soozangar N., Jeddi F., Mirzanejad-asl H., Molaei S., Habibzadeh S., Peeri doghaheh H., Mohammadshahi J., Spotin A.</t>
+  </si>
+  <si>
+    <t>Nurmakhanov T., Turebekov N., Tukhanova N., Turebekov N., Tukhanova N., Sadovskaya V., Tokmurziyeva G., Shevtsov A.</t>
+  </si>
+  <si>
+    <t>Jakimovski D., Banovic P., Urban P., Gorfol T., Lanszki Z., Tauber Z., Zana B., Banovic P., Zana B., Abraham A., Lanszki Z., Gorfol T., Tauber Z., Banovic P., Zana B., Abraham A., Lanszki Z., Gorfol T., Tauber Z., Kuczmog A., Banyai K., Spasovska K., Grozdanovski K., Rangelov G., Cvetanovska M., Cana F., Banovic P., Simin V., Bogdan I., Mijatovic D., Cvetkovikj A., Djadjovski I., Christova I., Meletis E., Kostoulas P., Zana B., Lanszki Z., Gorfol T., Tauber Z., Kemenesi G.</t>
+  </si>
+  <si>
+    <t>Bosevska G., Emmerich P., Von possel R., Toth E., Osmani D., Cadar D.</t>
+  </si>
+  <si>
+    <t>Marriott A., Berthet F., Nuttall P., Zeller H.</t>
+  </si>
+  <si>
+    <t>Parker M., Glass P., Jennings G., Lofts R., Smith J., Miller M., Glass P., Jennings G., Lofts R., Smith J., Miller M., Spik K., Schoepp R.</t>
   </si>
 </sst>
 </file>
@@ -1882,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1916,1491 +1916,1504 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>434</v>
+        <v>371</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>435</v>
+        <v>372</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>436</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>379</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>2015</v>
+        <v>261</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="6"/>
+        <v>262</v>
+      </c>
+      <c r="G2" s="5"/>
       <c r="H2" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>380</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>2024</v>
+        <v>194</v>
+      </c>
+      <c r="E3" t="s">
+        <v>195</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="I3" t="s">
-        <v>349</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>381</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>2019</v>
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>382</v>
+      </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" t="s">
+        <v>199</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>200</v>
+      </c>
+      <c r="G5" s="5"/>
       <c r="H5" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="I5" t="s">
-        <v>349</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>383</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>2021</v>
+        <v>278</v>
+      </c>
+      <c r="E6" t="s">
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="5">
-        <v>33416494</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>14</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>384</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>2020</v>
+        <v>257</v>
+      </c>
+      <c r="E7" t="s">
+        <v>258</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="5">
-        <v>33416494</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="H7" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="I7" t="s">
-        <v>349</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="E8">
-        <v>2022</v>
+        <v>2005</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>356</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>385</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9">
-        <v>2024</v>
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="6"/>
+        <v>128</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" t="s">
-        <v>357</v>
+        <v>321</v>
+      </c>
+      <c r="I9" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>386</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10">
-        <v>2019</v>
+        <v>245</v>
+      </c>
+      <c r="E10" t="s">
+        <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="5">
-        <v>33754998</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" t="s">
-        <v>358</v>
-      </c>
-      <c r="I10" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>387</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11">
-        <v>2024</v>
+        <v>179</v>
+      </c>
+      <c r="E11" t="s">
+        <v>180</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="6"/>
+        <v>181</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" t="s">
-        <v>359</v>
+        <v>336</v>
+      </c>
+      <c r="I11" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>388</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12">
-        <v>2023</v>
+        <v>237</v>
+      </c>
+      <c r="E12" t="s">
+        <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="6"/>
+        <v>238</v>
+      </c>
+      <c r="G12" s="5">
+        <v>19553586</v>
+      </c>
       <c r="H12" t="s">
-        <v>360</v>
+        <v>353</v>
+      </c>
+      <c r="I12" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>389</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13">
-        <v>2023</v>
+        <v>110</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>112</v>
+      </c>
+      <c r="G13" s="5">
+        <v>19523314</v>
+      </c>
       <c r="H13" t="s">
-        <v>361</v>
+        <v>316</v>
+      </c>
+      <c r="I13" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14">
-        <v>2013</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" t="s">
-        <v>362</v>
+        <v>291</v>
+      </c>
+      <c r="I14" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>390</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15">
-        <v>2024</v>
+        <v>220</v>
+      </c>
+      <c r="E15" t="s">
+        <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>221</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="H15" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>391</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16">
-        <v>2022</v>
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="G16" s="5">
+        <v>22119389</v>
+      </c>
       <c r="H16" t="s">
-        <v>364</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>392</v>
+      </c>
+      <c r="D17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" t="s">
+        <v>228</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" t="s">
-        <v>365</v>
-      </c>
-      <c r="I17" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>393</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18">
-        <v>2023</v>
+        <v>141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>375</v>
+      </c>
       <c r="H18" t="s">
-        <v>366</v>
+        <v>325</v>
+      </c>
+      <c r="I18" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>394</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19">
-        <v>2005</v>
+        <v>223</v>
+      </c>
+      <c r="E19" t="s">
+        <v>224</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="6"/>
+        <v>225</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>369</v>
+      </c>
       <c r="H19" t="s">
-        <v>367</v>
+        <v>349</v>
+      </c>
+      <c r="I19" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>395</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="6"/>
+        <v>192</v>
+      </c>
+      <c r="G20" s="5"/>
       <c r="H20" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>2013</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="5">
-        <v>38446223</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G21" s="6"/>
       <c r="H21" t="s">
-        <v>369</v>
-      </c>
-      <c r="I21" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>57</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>266</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>396</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>267</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>268</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="5">
-        <v>33388553</v>
+        <v>269</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>370</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>363</v>
       </c>
       <c r="I22" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>397</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>437</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>317</v>
       </c>
       <c r="I23" t="s">
-        <v>349</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>398</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="6"/>
+        <v>139</v>
+      </c>
+      <c r="G24" s="5">
+        <v>25108534</v>
+      </c>
       <c r="H24" t="s">
-        <v>370</v>
+        <v>324</v>
+      </c>
+      <c r="I24" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>399</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>243</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>244</v>
       </c>
       <c r="G25" s="5">
-        <v>31022170</v>
+        <v>33954213</v>
       </c>
       <c r="H25" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="I25" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>270</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>400</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>271</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="5">
-        <v>34662872</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="G26" s="5"/>
       <c r="H26" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="I26" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>2015</v>
       </c>
       <c r="F27" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" t="s">
-        <v>373</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>253</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>401</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>254</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>255</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>256</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>351</v>
+        <v>378</v>
       </c>
       <c r="H28" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="I28" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>71</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>402</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="G29" s="5">
-        <v>39565134</v>
+        <v>27523802</v>
       </c>
       <c r="H29" t="s">
-        <v>375</v>
-      </c>
-      <c r="I29" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>403</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="5">
-        <v>31291242</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="G30" s="5"/>
       <c r="H30" t="s">
-        <v>376</v>
+        <v>320</v>
       </c>
       <c r="I30" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>404</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="5">
-        <v>27926935</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="G31" s="6"/>
       <c r="H31" t="s">
-        <v>377</v>
-      </c>
-      <c r="I31" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>405</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="G32" s="5">
-        <v>22119389</v>
+        <v>27926935</v>
       </c>
       <c r="H32" t="s">
-        <v>378</v>
+        <v>314</v>
+      </c>
+      <c r="I32" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>406</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E33" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G33" s="5">
-        <v>19523314</v>
+        <v>28251517</v>
       </c>
       <c r="H33" t="s">
-        <v>379</v>
+        <v>319</v>
       </c>
       <c r="I33" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="G34" s="6"/>
       <c r="H34" t="s">
-        <v>380</v>
-      </c>
-      <c r="I34" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>407</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="G35" s="5">
-        <v>33142046</v>
+        <v>29148370</v>
       </c>
       <c r="H35" t="s">
-        <v>381</v>
+        <v>342</v>
       </c>
       <c r="I35" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>408</v>
+      </c>
+      <c r="D36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" t="s">
         <v>135</v>
       </c>
-      <c r="C36" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" t="s">
-        <v>137</v>
-      </c>
-      <c r="E36" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" t="s">
-        <v>138</v>
-      </c>
       <c r="G36" s="5">
-        <v>28251517</v>
+        <v>28902913</v>
       </c>
       <c r="H36" t="s">
-        <v>382</v>
+        <v>323</v>
       </c>
       <c r="I36" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>409</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>205</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F37" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>376</v>
+      </c>
       <c r="H37" t="s">
-        <v>383</v>
-      </c>
-      <c r="I37" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>410</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="F38" t="s">
-        <v>147</v>
-      </c>
-      <c r="G38" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="G38" s="5">
+        <v>31022170</v>
+      </c>
       <c r="H38" t="s">
-        <v>384</v>
+        <v>308</v>
       </c>
       <c r="I38" t="s">
-        <v>431</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>411</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="F39" t="s">
-        <v>150</v>
-      </c>
-      <c r="G39" s="5"/>
+        <v>167</v>
+      </c>
+      <c r="G39" s="5">
+        <v>31107219</v>
+      </c>
       <c r="H39" t="s">
-        <v>385</v>
+        <v>332</v>
       </c>
       <c r="I39" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>412</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" s="5">
-        <v>28902913</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G40" s="6"/>
       <c r="H40" t="s">
-        <v>386</v>
-      </c>
-      <c r="I40" t="s">
-        <v>350</v>
+        <v>310</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>250</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>413</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>251</v>
       </c>
       <c r="E41" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>160</v>
-      </c>
-      <c r="G41" s="5">
-        <v>25108534</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G41" s="6"/>
       <c r="H41" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
       <c r="I41" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>414</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>438</v>
+        <v>146</v>
+      </c>
+      <c r="G42" s="5">
+        <v>31211933</v>
       </c>
       <c r="H42" t="s">
-        <v>388</v>
+        <v>326</v>
       </c>
       <c r="I42" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>415</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="F43" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G43" s="5">
-        <v>31211933</v>
+        <v>32738065</v>
       </c>
       <c r="H43" t="s">
-        <v>389</v>
+        <v>330</v>
       </c>
       <c r="I43" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>416</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>173</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>174</v>
-      </c>
-      <c r="G44" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="G44" s="5">
+        <v>31291242</v>
+      </c>
       <c r="H44" t="s">
-        <v>390</v>
+        <v>313</v>
+      </c>
+      <c r="I44" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>176</v>
+        <v>417</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="E45" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="F45" t="s">
-        <v>179</v>
-      </c>
-      <c r="G45" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="G45" s="5">
+        <v>35551538</v>
+      </c>
       <c r="H45" t="s">
-        <v>391</v>
+        <v>346</v>
+      </c>
+      <c r="I45" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E46" t="s">
-        <v>70</v>
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>2019</v>
       </c>
       <c r="F46" t="s">
-        <v>183</v>
-      </c>
-      <c r="G46" s="5">
-        <v>40045205</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G46" s="5"/>
       <c r="H46" t="s">
-        <v>392</v>
+        <v>16</v>
       </c>
       <c r="I46" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>418</v>
       </c>
       <c r="D47" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>72</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
-      </c>
-      <c r="G47" s="5">
-        <v>32738065</v>
+        <v>213</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>377</v>
       </c>
       <c r="H47" t="s">
-        <v>393</v>
-      </c>
-      <c r="I47" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>189</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>190</v>
+        <v>419</v>
       </c>
       <c r="D48" t="s">
-        <v>191</v>
+        <v>117</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F48" t="s">
-        <v>192</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>347</v>
+        <v>118</v>
+      </c>
+      <c r="G48" s="5">
+        <v>33142046</v>
       </c>
       <c r="H48" t="s">
-        <v>394</v>
+        <v>318</v>
       </c>
       <c r="I48" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>193</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>420</v>
       </c>
       <c r="D49" t="s">
-        <v>195</v>
+        <v>71</v>
       </c>
       <c r="E49" t="s">
-        <v>187</v>
+        <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
       <c r="G49" s="5">
-        <v>31107219</v>
+        <v>33388553</v>
       </c>
       <c r="H49" t="s">
-        <v>395</v>
+        <v>74</v>
       </c>
       <c r="I49" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>198</v>
+        <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
-      </c>
-      <c r="E50" t="s">
-        <v>200</v>
+        <v>34</v>
+      </c>
+      <c r="E50">
+        <v>2019</v>
       </c>
       <c r="F50" t="s">
-        <v>201</v>
+        <v>35</v>
       </c>
       <c r="G50" s="5">
-        <v>33421655</v>
+        <v>33754998</v>
       </c>
       <c r="H50" t="s">
-        <v>396</v>
+        <v>295</v>
       </c>
       <c r="I50" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>202</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>203</v>
-      </c>
-      <c r="D51" t="s">
-        <v>204</v>
-      </c>
-      <c r="E51" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F51" t="s">
-        <v>205</v>
-      </c>
-      <c r="G51" s="5">
-        <v>39238565</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G51" s="5"/>
       <c r="H51" t="s">
-        <v>397</v>
+        <v>302</v>
       </c>
       <c r="I51" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
         <v>129</v>
       </c>
-      <c r="B52" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" t="s">
-        <v>207</v>
-      </c>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>130</v>
       </c>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F52" t="s">
-        <v>209</v>
-      </c>
-      <c r="G52" s="5">
-        <v>37766297</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="G52" s="5"/>
       <c r="H52" t="s">
-        <v>398</v>
+        <v>322</v>
       </c>
       <c r="I52" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
-        <v>211</v>
+        <v>421</v>
       </c>
       <c r="D53" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="E53" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="F53" t="s">
-        <v>214</v>
-      </c>
-      <c r="G53" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="G53" s="5">
+        <v>33421655</v>
+      </c>
       <c r="H53" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
       <c r="I53" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
       <c r="C54" t="s">
-        <v>216</v>
+        <v>422</v>
       </c>
       <c r="D54" t="s">
-        <v>217</v>
+        <v>264</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>218</v>
-      </c>
-      <c r="G54" s="6"/>
+        <v>265</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>285</v>
+      </c>
       <c r="H54" t="s">
-        <v>400</v>
+        <v>362</v>
+      </c>
+      <c r="I54" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>144</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>21</v>
       </c>
       <c r="D55" t="s">
-        <v>220</v>
-      </c>
-      <c r="E55" t="s">
-        <v>221</v>
+        <v>22</v>
+      </c>
+      <c r="E55">
+        <v>2021</v>
       </c>
       <c r="F55" t="s">
-        <v>222</v>
-      </c>
-      <c r="G55" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="G55" s="5">
+        <v>33416494</v>
+      </c>
       <c r="H55" t="s">
-        <v>401</v>
+        <v>24</v>
+      </c>
+      <c r="I55" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>145</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>224</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>225</v>
-      </c>
-      <c r="E56" t="s">
-        <v>226</v>
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>2020</v>
       </c>
       <c r="F56" t="s">
-        <v>227</v>
-      </c>
-      <c r="G56" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="G56" s="5">
+        <v>33416494</v>
+      </c>
       <c r="H56" t="s">
-        <v>402</v>
+        <v>292</v>
+      </c>
+      <c r="I56" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>228</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>423</v>
       </c>
       <c r="D57" t="s">
         <v>230</v>
@@ -3411,744 +3424,731 @@
       <c r="F57" t="s">
         <v>232</v>
       </c>
-      <c r="G57" s="6"/>
+      <c r="G57" s="5">
+        <v>35531170</v>
+      </c>
       <c r="H57" t="s">
-        <v>403</v>
-      </c>
-      <c r="I57" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>234</v>
+        <v>424</v>
       </c>
       <c r="D58" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>236</v>
+        <v>81</v>
       </c>
       <c r="F58" t="s">
-        <v>237</v>
-      </c>
-      <c r="G58" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="G58" s="5">
+        <v>33672497</v>
+      </c>
       <c r="H58" t="s">
-        <v>404</v>
+        <v>347</v>
       </c>
       <c r="I58" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>238</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>239</v>
+        <v>425</v>
       </c>
       <c r="D59" t="s">
-        <v>240</v>
+        <v>88</v>
       </c>
       <c r="E59" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="F59" t="s">
-        <v>241</v>
+        <v>89</v>
       </c>
       <c r="G59" s="5">
-        <v>29148370</v>
+        <v>34662872</v>
       </c>
       <c r="H59" t="s">
-        <v>405</v>
+        <v>309</v>
       </c>
       <c r="I59" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="B60" t="s">
-        <v>242</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>243</v>
+        <v>426</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>282</v>
       </c>
       <c r="F60" t="s">
-        <v>245</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>439</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="G60" s="5"/>
       <c r="H60" t="s">
-        <v>406</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>153</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>247</v>
+        <v>427</v>
       </c>
       <c r="D61" t="s">
-        <v>248</v>
+        <v>80</v>
       </c>
       <c r="E61" t="s">
-        <v>249</v>
+        <v>81</v>
       </c>
       <c r="F61" t="s">
-        <v>250</v>
-      </c>
-      <c r="G61" s="5">
-        <v>27523802</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="G61" s="6"/>
       <c r="H61" t="s">
-        <v>407</v>
+        <v>307</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>253</v>
-      </c>
-      <c r="E62" t="s">
-        <v>75</v>
+        <v>28</v>
+      </c>
+      <c r="E62">
+        <v>2022</v>
       </c>
       <c r="F62" t="s">
-        <v>254</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>440</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G62" s="6"/>
       <c r="H62" t="s">
-        <v>408</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>51</v>
       </c>
       <c r="D63" t="s">
-        <v>256</v>
-      </c>
-      <c r="E63" t="s">
-        <v>75</v>
+        <v>52</v>
+      </c>
+      <c r="E63">
+        <v>2022</v>
       </c>
       <c r="F63" t="s">
-        <v>257</v>
-      </c>
-      <c r="G63" s="5">
-        <v>35551538</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G63" s="5"/>
       <c r="H63" t="s">
-        <v>409</v>
-      </c>
-      <c r="I63" t="s">
-        <v>350</v>
+        <v>301</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="B64" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>428</v>
       </c>
       <c r="D64" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="E64" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F64" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="G64" s="5">
-        <v>33672497</v>
+        <v>37527191</v>
       </c>
       <c r="H64" t="s">
-        <v>410</v>
+        <v>365</v>
       </c>
       <c r="I64" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>262</v>
+        <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>263</v>
+        <v>429</v>
       </c>
       <c r="D65" t="s">
-        <v>264</v>
+        <v>163</v>
       </c>
       <c r="E65" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="F65" t="s">
-        <v>265</v>
-      </c>
-      <c r="G65" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="H65" t="s">
-        <v>411</v>
+        <v>331</v>
+      </c>
+      <c r="I65" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>160</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>267</v>
+        <v>430</v>
       </c>
       <c r="D66" t="s">
-        <v>268</v>
+        <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>269</v>
+        <v>77</v>
       </c>
       <c r="F66" t="s">
-        <v>270</v>
+        <v>78</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>432</v>
+        <v>374</v>
       </c>
       <c r="H66" t="s">
-        <v>412</v>
+        <v>79</v>
       </c>
       <c r="I66" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="B67" t="s">
-        <v>271</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>272</v>
+        <v>431</v>
       </c>
       <c r="D67" t="s">
-        <v>273</v>
+        <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>274</v>
+        <v>64</v>
       </c>
       <c r="F67" t="s">
-        <v>275</v>
-      </c>
-      <c r="G67" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="G67" s="6"/>
       <c r="H67" t="s">
-        <v>413</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="C68" t="s">
-        <v>276</v>
+        <v>432</v>
       </c>
       <c r="D68" t="s">
-        <v>277</v>
+        <v>176</v>
       </c>
       <c r="E68" t="s">
-        <v>278</v>
+        <v>68</v>
       </c>
       <c r="F68" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="G68" s="5">
-        <v>35531170</v>
+        <v>37766297</v>
       </c>
       <c r="H68" t="s">
-        <v>414</v>
+        <v>335</v>
+      </c>
+      <c r="I68" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>170</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>280</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>281</v>
+        <v>433</v>
       </c>
       <c r="D69" t="s">
-        <v>282</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>283</v>
+        <v>68</v>
       </c>
       <c r="F69" t="s">
-        <v>284</v>
+        <v>69</v>
       </c>
       <c r="G69" s="5">
-        <v>37879367</v>
+        <v>38446223</v>
       </c>
       <c r="H69" t="s">
-        <v>415</v>
+        <v>306</v>
       </c>
       <c r="I69" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>285</v>
+        <v>434</v>
       </c>
       <c r="D70" t="s">
-        <v>286</v>
+        <v>67</v>
       </c>
       <c r="E70" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="F70" t="s">
+        <v>94</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="H70" t="s">
+        <v>311</v>
+      </c>
+      <c r="I70" t="s">
         <v>287</v>
-      </c>
-      <c r="G70" s="5">
-        <v>19553586</v>
-      </c>
-      <c r="H70" t="s">
-        <v>416</v>
-      </c>
-      <c r="I70" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B71" t="s">
-        <v>288</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
-        <v>289</v>
+        <v>435</v>
       </c>
       <c r="D71" t="s">
-        <v>290</v>
+        <v>234</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>235</v>
       </c>
       <c r="F71" t="s">
-        <v>291</v>
-      </c>
-      <c r="G71" s="6"/>
+        <v>236</v>
+      </c>
+      <c r="G71" s="5">
+        <v>37879367</v>
+      </c>
       <c r="H71" t="s">
-        <v>417</v>
+        <v>352</v>
       </c>
       <c r="I71" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>177</v>
+        <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>292</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>293</v>
+        <v>56</v>
       </c>
       <c r="D72" t="s">
-        <v>294</v>
-      </c>
-      <c r="E72" t="s">
-        <v>249</v>
+        <v>57</v>
+      </c>
+      <c r="E72">
+        <v>2023</v>
       </c>
       <c r="F72" t="s">
-        <v>295</v>
-      </c>
-      <c r="G72" s="5">
-        <v>33954213</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G72" s="5"/>
       <c r="H72" t="s">
-        <v>418</v>
-      </c>
-      <c r="I72" t="s">
-        <v>350</v>
+        <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>180</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>296</v>
+        <v>436</v>
       </c>
       <c r="D73" t="s">
-        <v>297</v>
+        <v>156</v>
       </c>
       <c r="E73" t="s">
-        <v>298</v>
+        <v>68</v>
       </c>
       <c r="F73" t="s">
-        <v>299</v>
-      </c>
-      <c r="G73" s="5"/>
+        <v>157</v>
+      </c>
+      <c r="G73" s="5">
+        <v>40045205</v>
+      </c>
       <c r="H73" t="s">
-        <v>419</v>
+        <v>329</v>
+      </c>
+      <c r="I73" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="B74" t="s">
-        <v>300</v>
+        <v>172</v>
       </c>
       <c r="C74" t="s">
-        <v>301</v>
+        <v>437</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="E74" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="F74" t="s">
-        <v>302</v>
-      </c>
-      <c r="G74" s="6"/>
+        <v>174</v>
+      </c>
+      <c r="G74" s="5">
+        <v>39238565</v>
+      </c>
       <c r="H74" t="s">
-        <v>420</v>
+        <v>334</v>
+      </c>
+      <c r="I74" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>303</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>304</v>
+        <v>42</v>
       </c>
       <c r="D75" t="s">
-        <v>305</v>
-      </c>
-      <c r="E75" t="s">
-        <v>91</v>
+        <v>43</v>
+      </c>
+      <c r="E75">
+        <v>2023</v>
       </c>
       <c r="F75" t="s">
-        <v>306</v>
+        <v>44</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" t="s">
-        <v>421</v>
-      </c>
-      <c r="I75" t="s">
-        <v>349</v>
+        <v>298</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>188</v>
+        <v>34</v>
       </c>
       <c r="B76" t="s">
-        <v>307</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>308</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>309</v>
-      </c>
-      <c r="E76" t="s">
-        <v>310</v>
+        <v>40</v>
+      </c>
+      <c r="E76">
+        <v>2023</v>
       </c>
       <c r="F76" t="s">
-        <v>311</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>441</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G76" s="6"/>
       <c r="H76" t="s">
-        <v>422</v>
-      </c>
-      <c r="I76" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>190</v>
+        <v>18</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>312</v>
+        <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>313</v>
-      </c>
-      <c r="E77" t="s">
-        <v>314</v>
+        <v>31</v>
+      </c>
+      <c r="E77">
+        <v>2024</v>
       </c>
       <c r="F77" t="s">
-        <v>315</v>
+        <v>32</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" t="s">
-        <v>423</v>
-      </c>
-      <c r="I77" t="s">
-        <v>349</v>
+        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>191</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>316</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>317</v>
+        <v>48</v>
       </c>
       <c r="D78" t="s">
-        <v>318</v>
-      </c>
-      <c r="E78" t="s">
-        <v>231</v>
+        <v>49</v>
+      </c>
+      <c r="E78">
+        <v>2024</v>
       </c>
       <c r="F78" t="s">
-        <v>319</v>
-      </c>
-      <c r="G78" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="G78" s="6"/>
       <c r="H78" t="s">
-        <v>424</v>
+        <v>300</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>192</v>
+        <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>320</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>321</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>322</v>
-      </c>
-      <c r="E79" t="s">
-        <v>200</v>
+        <v>11</v>
+      </c>
+      <c r="E79">
+        <v>2024</v>
       </c>
       <c r="F79" t="s">
-        <v>323</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>348</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G79" s="6"/>
       <c r="H79" t="s">
-        <v>425</v>
+        <v>290</v>
       </c>
       <c r="I79" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>324</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s">
-        <v>325</v>
+        <v>438</v>
       </c>
       <c r="D80" t="s">
-        <v>326</v>
+        <v>240</v>
       </c>
       <c r="E80" t="s">
-        <v>327</v>
+        <v>97</v>
       </c>
       <c r="F80" t="s">
-        <v>328</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>433</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="G80" s="6"/>
       <c r="H80" t="s">
-        <v>426</v>
+        <v>354</v>
       </c>
       <c r="I80" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>195</v>
+        <v>71</v>
       </c>
       <c r="B81" t="s">
-        <v>329</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>330</v>
+        <v>439</v>
       </c>
       <c r="D81" t="s">
-        <v>331</v>
+        <v>96</v>
       </c>
       <c r="E81" t="s">
-        <v>332</v>
+        <v>97</v>
       </c>
       <c r="F81" t="s">
-        <v>333</v>
-      </c>
-      <c r="G81" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="G81" s="5">
+        <v>39565134</v>
+      </c>
       <c r="H81" t="s">
-        <v>427</v>
+        <v>312</v>
       </c>
       <c r="I81" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>197</v>
+        <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>334</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>335</v>
+        <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>336</v>
-      </c>
-      <c r="E82" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="E82">
+        <v>2024</v>
       </c>
       <c r="F82" t="s">
-        <v>337</v>
-      </c>
-      <c r="G82" s="5">
-        <v>37527191</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G82" s="6"/>
       <c r="H82" t="s">
-        <v>428</v>
-      </c>
-      <c r="I82" t="s">
-        <v>350</v>
+        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>338</v>
+        <v>147</v>
       </c>
       <c r="C83" t="s">
-        <v>339</v>
+        <v>440</v>
       </c>
       <c r="D83" t="s">
-        <v>340</v>
+        <v>148</v>
       </c>
       <c r="E83" t="s">
-        <v>341</v>
+        <v>149</v>
       </c>
       <c r="F83" t="s">
-        <v>342</v>
-      </c>
-      <c r="G83" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="G83" s="5"/>
       <c r="H83" t="s">
-        <v>429</v>
+        <v>327</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>208</v>
+        <v>144</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
+        <v>441</v>
       </c>
       <c r="D84" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="E84" t="s">
-        <v>345</v>
+        <v>187</v>
       </c>
       <c r="F84" t="s">
-        <v>346</v>
-      </c>
-      <c r="G84" s="5"/>
+        <v>188</v>
+      </c>
+      <c r="G84" s="6"/>
       <c r="H84" t="s">
-        <v>430</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I84" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
-      <sortCondition ref="A1:A84"/>
+      <sortCondition ref="F1:F84"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
remove non clinical from genbank, recognized by lab_host
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99078FD1-2B2B-AB4B-ABF3-85FFA437D69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9539A8-187A-9146-B951-A6746E1DA5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="500" windowWidth="25740" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="428">
   <si>
     <t>RefID</t>
   </si>
@@ -146,15 +146,6 @@
     <t>MN689741, MN689740, MN689739</t>
   </si>
   <si>
-    <t>Peng L., Hirsch S., Kocher G., Mehta M., Holbrook M.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IRF, NIH/NIAID, 8200 Research Plaza, Frederick, MD 21702, USA</t>
-  </si>
-  <si>
-    <t>PQ463984, PQ463983, PQ463982</t>
-  </si>
-  <si>
     <t>Picard C., Baize S.</t>
   </si>
   <si>
@@ -584,18 +575,6 @@
     <t>EF432639, EF432640, EF432641, EF432642, EF432643, EF432644, EF432645, EF432646, EF432647, EF432648, EF432649, EF432650, EF432651, EF432652, EF432653</t>
   </si>
   <si>
-    <t>Ap92 sequencing</t>
-  </si>
-  <si>
-    <t>Papa A., Papadopoulou E., Pappa S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MICROBIOLOGY, AUTH, AUTH CAMPUS, 54124, GREECE, Unpublished</t>
-  </si>
-  <si>
-    <t>LT673890</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Michael D. Parker, Virology Divison, USAMRIID, Bldg. 1425 Fort Detrick, Frederick, MD 21702, USA</t>
   </si>
   <si>
@@ -693,15 +672,6 @@
   </si>
   <si>
     <t>MW452933, MW452934, MW452935</t>
-  </si>
-  <si>
-    <t>The characterization of crimean-congo haemorrhagic fever virus glycoproteins, The crimean-congo haemorrhagic fever virus genetic analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Molecular Virology Lab, Wuhan Institution of Virology, CAS, No. 44, Xiaohongshan Middle District, Wuchan District, Wuhan, Hubei 430071, China, Unpublished</t>
-  </si>
-  <si>
-    <t>FJ562093, FJ562094, FJ562095</t>
   </si>
   <si>
     <t>A focal outbreak of crimean congo hemorrhagic fever in ahmadabad, india, 2011</t>
@@ -932,9 +902,6 @@
   </si>
   <si>
     <t xml:space="preserve">The GenBank submissions with accession numbers MN689741, MN689740, and MN689739 are associated with the study titled "Fatal Case of Crimean-Congo Hemorrhagic Fever Caused by Reassortant Virus, Spain, 2018," authored by Anabel Negredo, Rafael Sánchez-Arroyo, Francisco Díez-Fuertes, Fernando de Ory, Marco Antonio Budiño, Ana Vázquez, Ángeles Garcinuño, Lourdes Hernández, César de la Hoz González, Almudena Gutiérrez-Arroyo, Carmen Grande, and Paz Sánchez-Seco. This study was published in the journal *Emerging Infectious Diseases* in April 2021. The PubMed Central ID (PMCID) for this article is PMC8007309, and the PubMed ID (PMID) is 33754998. ([pmc.ncbi.nlm.nih.gov](https://pmc.ncbi.nlm.nih.gov/articles/PMC8007309/?utm_source=openai)) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I was unable to locate a publication associated with the GenBank submissions PQ463984, PQ463983, and PQ463982 by authors Peng L., Hirsch S., Kocher G., Mehta M., and Holbrook M. from the IRF, NIH/NIAID, Frederick, MD, USA, submitted in 2024. It's possible that the study has not been published yet or is not indexed in the databases searched. </t>
   </si>
   <si>
     <t xml:space="preserve">I searched for publications by C. Picard and S. Baize from the Virology department at Institut Pasteur, Lyon, France, in 2023, related to Crimean–Congo hemorrhagic fever virus, but I couldn't find any associated publications. It's possible that the study corresponding to the GenBank submissions with accession numbers PP067047 to PP067088 has not been published yet or is not indexed in the databases I searched. </t>
@@ -1110,9 +1077,6 @@
 **Year:** 2008
 **DOI:** [10.1007/s00705-007-1056-4](https://doi.org/10.1007/s00705-007-1056-4)
 This study focuses on the genetic analysis of the M RNA segment of Crimean-Congo hemorrhagic fever virus strains in Turkey. The inclusion of authors Aydin K., Koksal I., Ozdarendeli A., and Tonbak S., along with the 2007 submission date, suggests a strong association with the GenBank entries in question. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I was unable to locate a published study associated with the GenBank submission titled "Ap92 sequencing" by authors Papa A., Papadopoulou E., and Pappa S., submitted in 2016 with accession number LT673890. The submission is listed as unpublished in the GenBank database. It's possible that the study has not been published or is not indexed in the databases searched. </t>
   </si>
   <si>
     <t xml:space="preserve">The GenBank accession number U39455 corresponds to a sequence submitted by Michael D. Parker from the Virology Division at USAMRIID in 1995. However, there is no direct evidence linking this submission to a specific publication. The available information does not provide a clear connection to a published study associated with this GenBank entry. </t>
@@ -1171,9 +1135,6 @@
 The full text is available at: [https://www.mdpi.com/2076-2607/9/2/438](https://www.mdpi.com/2076-2607/9/2/438) </t>
   </si>
   <si>
-    <t xml:space="preserve">I was unable to locate a published study corresponding to the 2008 GenBank submissions titled "The characterization of Crimean-Congo haemorrhagic fever virus glycoproteins" and "The Crimean-Congo haemorrhagic fever virus genetic analysis" by Deng F., Hu Z., Li T., Meng W., Sun S., Wang H., Xia Y., Zhang Y., and Zhou Z. The GenBank entries (accessions FJ562093, FJ562094, FJ562095) are listed as unpublished. Therefore, it appears that these sequences have not been associated with a formal publication. </t>
-  </si>
-  <si>
     <t xml:space="preserve">The GenBank submissions titled "A focal outbreak of Crimean-Congo hemorrhagic fever in Ahmedabad, India, 2011" by authors Mourya D. and Yadav P., with accession numbers JF922673 to JF922681, are associated with the following publication:
 **Title:** Detection, isolation and confirmation of Crimean-Congo hemorrhagic fever virus in human, ticks and animals in Ahmadabad, India, 2010–2011
 **Authors:** Mourya DT, Yadav PD, Shete AM, Gurav YK, Raut CG, Jadi RS, Pawar SD, Nichol ST, Mishra AC
@@ -1320,9 +1281,6 @@
   </si>
   <si>
     <t>Carletti F., Di caro A., Capobianchi M., Castilletti C., Bordi L., Lalle E., Castilletti C., Capobianchi M., Ippolito G., Bordi L., Lalle E., Chiappini R.</t>
-  </si>
-  <si>
-    <t>Xia Y., Zhou Z., Meng W., Hu Z., Wang H., Zhang Y., Sun S., Li T., Hu Z., Wang H., Deng F.</t>
   </si>
   <si>
     <t>Bursali A., Tekin S., Mutluay N., Ekici M., Ozkan M., Dundar E.</t>
@@ -1880,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1916,326 +1874,326 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I3" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" t="s">
-        <v>381</v>
-      </c>
-      <c r="D4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" t="s">
-        <v>154</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="I5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="D6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E6" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="F6" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="I7" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8">
         <v>2005</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
         <v>125</v>
-      </c>
-      <c r="C9" t="s">
-        <v>385</v>
-      </c>
-      <c r="D9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" t="s">
-        <v>128</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="I9" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="E10" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" t="s">
+        <v>374</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" t="s">
         <v>178</v>
-      </c>
-      <c r="C11" t="s">
-        <v>387</v>
-      </c>
-      <c r="D11" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" t="s">
-        <v>180</v>
-      </c>
-      <c r="F11" t="s">
-        <v>181</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="I11" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="D12" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="G12" s="5">
         <v>19553586</v>
       </c>
       <c r="H12" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="I12" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G13" s="5">
         <v>19523314</v>
       </c>
       <c r="H13" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="I13" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2253,1423 +2211,1428 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I14" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>104</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>221</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G15" s="5">
+        <v>22119389</v>
+      </c>
       <c r="H15" t="s">
-        <v>348</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="5">
-        <v>22119389</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G16" s="5"/>
       <c r="H16" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>139</v>
       </c>
       <c r="F17" t="s">
-        <v>229</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>362</v>
+      </c>
       <c r="H17" t="s">
-        <v>350</v>
+        <v>314</v>
+      </c>
+      <c r="I17" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="H18" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="I18" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="D19" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="E19" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="F19" t="s">
-        <v>225</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>369</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="G19" s="5"/>
       <c r="H19" t="s">
-        <v>349</v>
-      </c>
-      <c r="I19" t="s">
-        <v>287</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>395</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" t="s">
-        <v>191</v>
+        <v>43</v>
+      </c>
+      <c r="E20">
+        <v>2013</v>
       </c>
       <c r="F20" t="s">
-        <v>192</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="G20" s="6"/>
       <c r="H20" t="s">
-        <v>339</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>256</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>382</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21">
-        <v>2013</v>
+        <v>257</v>
+      </c>
+      <c r="E21" t="s">
+        <v>258</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>259</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>357</v>
+      </c>
       <c r="H21" t="s">
-        <v>299</v>
+        <v>350</v>
+      </c>
+      <c r="I21" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>194</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>266</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="D22" t="s">
-        <v>267</v>
+        <v>110</v>
       </c>
       <c r="E22" t="s">
-        <v>268</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
-        <v>269</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>370</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" t="s">
-        <v>363</v>
+        <v>306</v>
       </c>
       <c r="I22" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="E23" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="F23" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="G23" s="5">
+        <v>25108534</v>
+      </c>
       <c r="H23" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I23" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>112</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>232</v>
       </c>
       <c r="C24" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="G24" s="5">
-        <v>25108534</v>
+        <v>33954213</v>
       </c>
       <c r="H24" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="I24" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C25" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="D25" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="E25" t="s">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="F25" t="s">
-        <v>244</v>
-      </c>
-      <c r="G25" s="5">
-        <v>33954213</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="G25" s="5"/>
       <c r="H25" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="I25" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>195</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>400</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>271</v>
-      </c>
-      <c r="E26" t="s">
-        <v>272</v>
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>2015</v>
       </c>
       <c r="F26" t="s">
-        <v>273</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G26" s="6"/>
       <c r="H26" t="s">
-        <v>364</v>
-      </c>
-      <c r="I26" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>387</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27">
-        <v>2015</v>
+        <v>244</v>
+      </c>
+      <c r="E27" t="s">
+        <v>245</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="6"/>
+        <v>246</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>365</v>
+      </c>
       <c r="H27" t="s">
-        <v>289</v>
+        <v>346</v>
+      </c>
+      <c r="I27" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>253</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="D28" t="s">
-        <v>254</v>
+        <v>201</v>
       </c>
       <c r="E28" t="s">
-        <v>255</v>
+        <v>202</v>
       </c>
       <c r="F28" t="s">
-        <v>256</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>378</v>
+        <v>203</v>
+      </c>
+      <c r="G28" s="5">
+        <v>27523802</v>
       </c>
       <c r="H28" t="s">
-        <v>359</v>
-      </c>
-      <c r="I28" t="s">
-        <v>286</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
+        <v>120</v>
       </c>
       <c r="E29" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
-      </c>
-      <c r="G29" s="5">
-        <v>27523802</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" t="s">
-        <v>344</v>
+        <v>309</v>
+      </c>
+      <c r="I29" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>106</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>238</v>
       </c>
       <c r="C30" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>239</v>
+      </c>
+      <c r="G30" s="6"/>
       <c r="H30" t="s">
-        <v>320</v>
-      </c>
-      <c r="I30" t="s">
-        <v>286</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F31" t="s">
-        <v>249</v>
-      </c>
-      <c r="G31" s="6"/>
+        <v>102</v>
+      </c>
+      <c r="G31" s="5">
+        <v>27926935</v>
+      </c>
       <c r="H31" t="s">
-        <v>357</v>
+        <v>303</v>
+      </c>
+      <c r="I31" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="G32" s="5">
-        <v>27926935</v>
+        <v>28251517</v>
       </c>
       <c r="H32" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I32" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>194</v>
       </c>
       <c r="C33" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="G33" s="5">
-        <v>28251517</v>
+        <v>29148370</v>
       </c>
       <c r="H33" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="I33" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>183</v>
+        <v>394</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
-        <v>185</v>
-      </c>
-      <c r="G34" s="6"/>
+        <v>132</v>
+      </c>
+      <c r="G34" s="5">
+        <v>28902913</v>
+      </c>
       <c r="H34" t="s">
-        <v>337</v>
+        <v>312</v>
+      </c>
+      <c r="I34" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E35" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
-      </c>
-      <c r="G35" s="5">
-        <v>29148370</v>
+        <v>199</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>363</v>
       </c>
       <c r="H35" t="s">
-        <v>342</v>
-      </c>
-      <c r="I35" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="G36" s="5">
-        <v>28902913</v>
+        <v>31022170</v>
       </c>
       <c r="H36" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="I36" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D37" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="F37" t="s">
-        <v>206</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>376</v>
+        <v>164</v>
+      </c>
+      <c r="G37" s="5">
+        <v>31107219</v>
       </c>
       <c r="H37" t="s">
-        <v>343</v>
+        <v>321</v>
+      </c>
+      <c r="I37" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="5">
-        <v>31022170</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="G38" s="6"/>
       <c r="H38" t="s">
-        <v>308</v>
-      </c>
-      <c r="I38" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="C39" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>241</v>
       </c>
       <c r="E39" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="F39" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39" s="5">
-        <v>31107219</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="G39" s="6"/>
       <c r="H39" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="I39" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F40" t="s">
-        <v>92</v>
-      </c>
-      <c r="G40" s="6"/>
+        <v>143</v>
+      </c>
+      <c r="G40" s="5">
+        <v>31211933</v>
+      </c>
       <c r="H40" t="s">
-        <v>310</v>
+        <v>315</v>
+      </c>
+      <c r="I40" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="C41" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="D41" t="s">
-        <v>251</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
-        <v>252</v>
-      </c>
-      <c r="G41" s="6"/>
+        <v>158</v>
+      </c>
+      <c r="G41" s="5">
+        <v>32738065</v>
+      </c>
       <c r="H41" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="I41" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="E42" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F42" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="G42" s="5">
-        <v>31211933</v>
+        <v>31291242</v>
       </c>
       <c r="H42" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="I42" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="E43" t="s">
-        <v>160</v>
+        <v>69</v>
       </c>
       <c r="F43" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="G43" s="5">
-        <v>32738065</v>
+        <v>35551538</v>
       </c>
       <c r="H43" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="I43" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>416</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" t="s">
-        <v>72</v>
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>2019</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
-      </c>
-      <c r="G44" s="5">
-        <v>31291242</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G44" s="5"/>
       <c r="H44" t="s">
-        <v>313</v>
+        <v>16</v>
       </c>
       <c r="I44" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="C45" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="D45" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F45" t="s">
-        <v>215</v>
-      </c>
-      <c r="G45" s="5">
-        <v>35551538</v>
+        <v>206</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>364</v>
       </c>
       <c r="H45" t="s">
-        <v>346</v>
-      </c>
-      <c r="I45" t="s">
-        <v>287</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>405</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46">
-        <v>2019</v>
+        <v>114</v>
+      </c>
+      <c r="E46" t="s">
+        <v>69</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="G46" s="5">
+        <v>33142046</v>
+      </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I46" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="D47" t="s">
-        <v>212</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F47" t="s">
-        <v>213</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>377</v>
+        <v>70</v>
+      </c>
+      <c r="G47" s="5">
+        <v>33388553</v>
       </c>
       <c r="H47" t="s">
-        <v>345</v>
+        <v>71</v>
+      </c>
+      <c r="I47" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>419</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>117</v>
-      </c>
-      <c r="E48" t="s">
-        <v>72</v>
+        <v>34</v>
+      </c>
+      <c r="E48">
+        <v>2019</v>
       </c>
       <c r="F48" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="G48" s="5">
-        <v>33142046</v>
+        <v>33754998</v>
       </c>
       <c r="H48" t="s">
-        <v>318</v>
+        <v>285</v>
       </c>
       <c r="I48" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>420</v>
-      </c>
-      <c r="D49" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F49" t="s">
-        <v>73</v>
-      </c>
-      <c r="G49" s="5">
-        <v>33388553</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G49" s="5"/>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="I49" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50">
-        <v>2019</v>
+        <v>127</v>
+      </c>
+      <c r="E50" t="s">
+        <v>69</v>
       </c>
       <c r="F50" t="s">
-        <v>35</v>
-      </c>
-      <c r="G50" s="5">
-        <v>33754998</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G50" s="5"/>
       <c r="H50" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="I50" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>407</v>
+      </c>
+      <c r="D51" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" t="s">
+        <v>167</v>
       </c>
       <c r="F51" t="s">
-        <v>35</v>
-      </c>
-      <c r="G51" s="5"/>
+        <v>168</v>
+      </c>
+      <c r="G51" s="5">
+        <v>33421655</v>
+      </c>
       <c r="H51" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="I51" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>253</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>408</v>
       </c>
       <c r="D52" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>167</v>
       </c>
       <c r="F52" t="s">
-        <v>131</v>
-      </c>
-      <c r="G52" s="5"/>
+        <v>255</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="H52" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="I52" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>421</v>
+        <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
-      </c>
-      <c r="E53" t="s">
-        <v>170</v>
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>2021</v>
       </c>
       <c r="F53" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="G53" s="5">
-        <v>33421655</v>
+        <v>33416494</v>
       </c>
       <c r="H53" t="s">
-        <v>333</v>
+        <v>24</v>
       </c>
       <c r="I53" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>263</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>422</v>
+        <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>264</v>
-      </c>
-      <c r="E54" t="s">
-        <v>170</v>
+        <v>26</v>
+      </c>
+      <c r="E54">
+        <v>2020</v>
       </c>
       <c r="F54" t="s">
-        <v>265</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>285</v>
+        <v>23</v>
+      </c>
+      <c r="G54" s="5">
+        <v>33416494</v>
       </c>
       <c r="H54" t="s">
-        <v>362</v>
+        <v>282</v>
       </c>
       <c r="I54" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>409</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55">
-        <v>2021</v>
+        <v>220</v>
+      </c>
+      <c r="E55" t="s">
+        <v>221</v>
       </c>
       <c r="F55" t="s">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="G55" s="5">
-        <v>33416494</v>
+        <v>35531170</v>
       </c>
       <c r="H55" t="s">
-        <v>24</v>
-      </c>
-      <c r="I55" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>410</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
-      </c>
-      <c r="E56">
-        <v>2020</v>
+        <v>210</v>
+      </c>
+      <c r="E56" t="s">
+        <v>78</v>
       </c>
       <c r="F56" t="s">
-        <v>23</v>
+        <v>211</v>
       </c>
       <c r="G56" s="5">
-        <v>33416494</v>
+        <v>33672497</v>
       </c>
       <c r="H56" t="s">
-        <v>292</v>
+        <v>335</v>
       </c>
       <c r="I56" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>166</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="D57" t="s">
-        <v>230</v>
+        <v>85</v>
       </c>
       <c r="E57" t="s">
-        <v>231</v>
+        <v>78</v>
       </c>
       <c r="F57" t="s">
-        <v>232</v>
+        <v>86</v>
       </c>
       <c r="G57" s="5">
-        <v>35531170</v>
+        <v>34662872</v>
       </c>
       <c r="H57" t="s">
-        <v>351</v>
+        <v>298</v>
+      </c>
+      <c r="I57" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>158</v>
+        <v>203</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D58" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>272</v>
       </c>
       <c r="F58" t="s">
-        <v>218</v>
-      </c>
-      <c r="G58" s="5">
-        <v>33672497</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="G58" s="5"/>
       <c r="H58" t="s">
-        <v>347</v>
-      </c>
-      <c r="I58" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D59" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F59" t="s">
-        <v>89</v>
-      </c>
-      <c r="G59" s="5">
-        <v>34662872</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G59" s="6"/>
       <c r="H59" t="s">
-        <v>309</v>
-      </c>
-      <c r="I59" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>208</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>426</v>
+        <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>281</v>
-      </c>
-      <c r="E60" t="s">
-        <v>282</v>
+        <v>28</v>
+      </c>
+      <c r="E60">
+        <v>2022</v>
       </c>
       <c r="F60" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" t="s">
         <v>283</v>
-      </c>
-      <c r="G60" s="5"/>
-      <c r="H60" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>427</v>
+        <v>48</v>
       </c>
       <c r="D61" t="s">
-        <v>80</v>
-      </c>
-      <c r="E61" t="s">
-        <v>81</v>
+        <v>49</v>
+      </c>
+      <c r="E61">
+        <v>2022</v>
       </c>
       <c r="F61" t="s">
-        <v>82</v>
-      </c>
-      <c r="G61" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="G61" s="5"/>
       <c r="H61" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>414</v>
       </c>
       <c r="D62" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62">
-        <v>2022</v>
+        <v>265</v>
+      </c>
+      <c r="E62" t="s">
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>29</v>
-      </c>
-      <c r="G62" s="6"/>
+        <v>266</v>
+      </c>
+      <c r="G62" s="5">
+        <v>37527191</v>
+      </c>
       <c r="H62" t="s">
-        <v>293</v>
+        <v>352</v>
+      </c>
+      <c r="I62" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>415</v>
       </c>
       <c r="D63" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63">
-        <v>2022</v>
+        <v>160</v>
+      </c>
+      <c r="E63" t="s">
+        <v>74</v>
       </c>
       <c r="F63" t="s">
-        <v>53</v>
-      </c>
-      <c r="G63" s="5"/>
+        <v>161</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="H63" t="s">
-        <v>301</v>
+        <v>320</v>
+      </c>
+      <c r="I63" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>274</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D64" t="s">
-        <v>275</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F64" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H64" t="s">
+        <v>76</v>
+      </c>
+      <c r="I64" t="s">
         <v>276</v>
-      </c>
-      <c r="G64" s="5">
-        <v>37527191</v>
-      </c>
-      <c r="H64" t="s">
-        <v>365</v>
-      </c>
-      <c r="I64" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>162</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D65" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F65" t="s">
-        <v>164</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>284</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G65" s="6"/>
       <c r="H65" t="s">
-        <v>331</v>
-      </c>
-      <c r="I65" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="C66" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>173</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F66" t="s">
-        <v>78</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>374</v>
+        <v>174</v>
+      </c>
+      <c r="G66" s="5">
+        <v>37766297</v>
       </c>
       <c r="H66" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="I66" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3677,480 +3640,399 @@
         <v>54</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D67" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F67" t="s">
-        <v>65</v>
-      </c>
-      <c r="G67" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="G67" s="5">
+        <v>38446223</v>
+      </c>
       <c r="H67" t="s">
-        <v>305</v>
+        <v>295</v>
+      </c>
+      <c r="I67" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>175</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D68" t="s">
-        <v>176</v>
+        <v>64</v>
       </c>
       <c r="E68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F68" t="s">
-        <v>177</v>
-      </c>
-      <c r="G68" s="5">
-        <v>37766297</v>
+        <v>91</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>278</v>
       </c>
       <c r="H68" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
       <c r="I68" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="C69" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="D69" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
       <c r="E69" t="s">
-        <v>68</v>
+        <v>225</v>
       </c>
       <c r="F69" t="s">
-        <v>69</v>
+        <v>226</v>
       </c>
       <c r="G69" s="5">
-        <v>38446223</v>
+        <v>37879367</v>
       </c>
       <c r="H69" t="s">
-        <v>306</v>
+        <v>339</v>
       </c>
       <c r="I69" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B70" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>434</v>
+        <v>53</v>
       </c>
       <c r="D70" t="s">
-        <v>67</v>
-      </c>
-      <c r="E70" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="E70">
+        <v>2023</v>
       </c>
       <c r="F70" t="s">
-        <v>94</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>288</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G70" s="5"/>
       <c r="H70" t="s">
-        <v>311</v>
-      </c>
-      <c r="I70" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>233</v>
+        <v>152</v>
       </c>
       <c r="C71" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="D71" t="s">
-        <v>234</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>65</v>
       </c>
       <c r="F71" t="s">
-        <v>236</v>
+        <v>154</v>
       </c>
       <c r="G71" s="5">
-        <v>37879367</v>
+        <v>40045205</v>
       </c>
       <c r="H71" t="s">
-        <v>352</v>
+        <v>318</v>
       </c>
       <c r="I71" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C72" t="s">
-        <v>56</v>
+        <v>423</v>
       </c>
       <c r="D72" t="s">
-        <v>57</v>
-      </c>
-      <c r="E72">
-        <v>2023</v>
+        <v>170</v>
+      </c>
+      <c r="E72" t="s">
+        <v>65</v>
       </c>
       <c r="F72" t="s">
-        <v>58</v>
-      </c>
-      <c r="G72" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="G72" s="5">
+        <v>39238565</v>
+      </c>
       <c r="H72" t="s">
-        <v>303</v>
+        <v>323</v>
+      </c>
+      <c r="I72" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="B73" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>436</v>
+        <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
-      </c>
-      <c r="E73" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="E73">
+        <v>2023</v>
       </c>
       <c r="F73" t="s">
-        <v>157</v>
-      </c>
-      <c r="G73" s="5">
-        <v>40045205</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G73" s="6"/>
       <c r="H73" t="s">
-        <v>329</v>
-      </c>
-      <c r="I73" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>172</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>437</v>
+        <v>36</v>
       </c>
       <c r="D74" t="s">
-        <v>173</v>
-      </c>
-      <c r="E74" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="E74">
+        <v>2023</v>
       </c>
       <c r="F74" t="s">
-        <v>174</v>
-      </c>
-      <c r="G74" s="5">
-        <v>39238565</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G74" s="6"/>
       <c r="H74" t="s">
-        <v>334</v>
-      </c>
-      <c r="I74" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E75">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E76">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F76" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E77">
         <v>2024</v>
       </c>
       <c r="F77" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" t="s">
-        <v>294</v>
+        <v>280</v>
+      </c>
+      <c r="I77" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>37</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>48</v>
+        <v>424</v>
       </c>
       <c r="D78" t="s">
-        <v>49</v>
-      </c>
-      <c r="E78">
-        <v>2024</v>
+        <v>230</v>
+      </c>
+      <c r="E78" t="s">
+        <v>94</v>
       </c>
       <c r="F78" t="s">
-        <v>50</v>
+        <v>231</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" t="s">
-        <v>300</v>
+        <v>341</v>
+      </c>
+      <c r="I78" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>425</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79">
-        <v>2024</v>
+        <v>93</v>
+      </c>
+      <c r="E79" t="s">
+        <v>94</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="G79" s="5">
+        <v>39565134</v>
+      </c>
       <c r="H79" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="I79" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>239</v>
+        <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="D80" t="s">
-        <v>240</v>
+        <v>145</v>
       </c>
       <c r="E80" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="F80" t="s">
-        <v>241</v>
-      </c>
-      <c r="G80" s="6"/>
+        <v>147</v>
+      </c>
+      <c r="G80" s="5"/>
       <c r="H80" t="s">
-        <v>354</v>
-      </c>
-      <c r="I80" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="D81" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="E81" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="F81" t="s">
-        <v>98</v>
-      </c>
-      <c r="G81" s="5">
-        <v>39565134</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="G81" s="6"/>
       <c r="H81" t="s">
-        <v>312</v>
-      </c>
-      <c r="I81" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>33</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>36</v>
-      </c>
-      <c r="D82" t="s">
-        <v>37</v>
-      </c>
-      <c r="E82">
-        <v>2024</v>
-      </c>
-      <c r="F82" t="s">
-        <v>38</v>
-      </c>
-      <c r="G82" s="6"/>
-      <c r="H82" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>116</v>
-      </c>
-      <c r="B83" t="s">
-        <v>147</v>
-      </c>
-      <c r="C83" t="s">
-        <v>440</v>
-      </c>
-      <c r="D83" t="s">
-        <v>148</v>
-      </c>
-      <c r="E83" t="s">
-        <v>149</v>
-      </c>
-      <c r="F83" t="s">
-        <v>150</v>
-      </c>
-      <c r="G83" s="5"/>
-      <c r="H83" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>144</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" t="s">
-        <v>441</v>
-      </c>
-      <c r="D84" t="s">
-        <v>186</v>
-      </c>
-      <c r="E84" t="s">
-        <v>187</v>
-      </c>
-      <c r="F84" t="s">
-        <v>188</v>
-      </c>
-      <c r="G84" s="6"/>
-      <c r="H84" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I84" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
-      <sortCondition ref="F1:F84"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
update the order of accession number for submission sets.
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9539A8-187A-9146-B951-A6746E1DA5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392F8A22-FB7F-B54F-B5F1-DF004DCB8D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="500" windowWidth="25740" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,18 +65,12 @@
     <t xml:space="preserve"> Virology, Public Health Institution of Turkey, Saglik Mahallesi Prof. Dr. Nusret Fisek Cad, Ankara, Sihhiye 06100, Turkey</t>
   </si>
   <si>
-    <t>KT266848, KT266847, KT266846, KT266845, KT266844, KT266843, KT266842, KT266841, KT266840, KT266839, KT266838, KT266837, KT266836, KT266835, KT266834, KT266833, KT266832</t>
-  </si>
-  <si>
     <t>Baz-flores S., Herrero G., Cuadrado-matias R., Moraga fernandez A., Peralbo-moreno A., Fernandez de mera I., Ruiz-fons F.</t>
   </si>
   <si>
     <t xml:space="preserve"> Sanidad Animal, Instituto de Investigacion en Recursos Cinegeticos, Ronda de Toledo s/n, Ciudad Real, Ciudad Real 13003, Espana</t>
   </si>
   <si>
-    <t>PP449386, PP449385, PP449384, PP449383, PP449382</t>
-  </si>
-  <si>
     <t>Chitimia-dobler L.</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>bioRxiv (2021) In press</t>
   </si>
   <si>
-    <t>MW058030, MW058029, MW058028</t>
-  </si>
-  <si>
     <t xml:space="preserve">The publication associated with the GenBank accessions MW058030, MW058029, and MW058028 is titled "Immunocompetent Mouse Model for Crimean-Congo Hemorrhagic Fever Virus" by authors David W. Hawman, Kimberly Meade-White, Shanna Leventhal, Friederike Feldmann, Atsushi Okumura, Brian Smith, Dana Scott, and Heinz Feldmann. It was published in *eLife* on January 8, 2021. The PubMed ID (PMID) for this article is 33416494. ([pubmed.ncbi.nlm.nih.gov](https://pubmed.ncbi.nlm.nih.gov/33416494/?utm_source=openai)) </t>
   </si>
   <si>
@@ -125,45 +116,30 @@
     <t xml:space="preserve"> Key Laboratory of Etiology and Epidemiology of Emerging Infectious Diseases, Shandong First Medical University and Shandong Academy of Medical Sciences, Yingshengdonglu No. 2, Taian 271000, China</t>
   </si>
   <si>
-    <t>ON500502, ON500501, ON500500</t>
-  </si>
-  <si>
     <t>Karan L., Perekopskaya N., Morozkin E., Roev G.</t>
   </si>
   <si>
     <t xml:space="preserve"> Department of Molecular Diagnostic and Epidemiology, Central Research Institute of Epidemiology, Novogireevskaya 3A, Moscow 111123, Russia</t>
   </si>
   <si>
-    <t>PP116320, PP116319, PP116318</t>
-  </si>
-  <si>
     <t>Negredo A., Vazquez A., Hernandez L., Sanchez-seco M.</t>
   </si>
   <si>
     <t xml:space="preserve"> Arbovirus and Imported Viral diseases, National Center of Microbiology, Institute of Health Carlos III, Ctra. Majadahonda-Pozuelo, km2, Majadahonda, Madrid 28220, Spain</t>
   </si>
   <si>
-    <t>MN689741, MN689740, MN689739</t>
-  </si>
-  <si>
     <t>Picard C., Baize S.</t>
   </si>
   <si>
     <t xml:space="preserve"> Virology, Institut Pasteur, 21 Av Tony Garnier, Lyon 69365, France</t>
   </si>
   <si>
-    <t>PP067088, PP067087, PP067086, PP067085, PP067084, PP067083, PP067082, PP067081, PP067080, PP067079, PP067078, PP067077, PP067076, PP067075, PP067074, PP067073, PP067072, PP067071, PP067070, PP067069, PP067068, PP067067, PP067066, PP067065, PP067064, PP067063, PP067062, PP067061, PP067060, PP067059, PP067058, PP067057, PP067056, PP067055, PP067054, PP067053, PP067052, PP067051, PP067050, PP067049, PP067048, PP067047</t>
-  </si>
-  <si>
     <t>Piorkowski G., Kiwan P., Masse S., Ayhan N., Charrel R., De lamballerie X., Falchi A.</t>
   </si>
   <si>
     <t xml:space="preserve"> UMR190 Unite des Virus Emergents U1207, IHU mediterranee, 19-21 boulevard Jean Moulin, Marseille 13005, France</t>
   </si>
   <si>
-    <t>PP025040, PP025039, PP025038</t>
-  </si>
-  <si>
     <t>Rangunwala A., Burt F., Swanepoel R., Janusz P.</t>
   </si>
   <si>
@@ -179,9 +155,6 @@
     <t xml:space="preserve"> Labaratory of Veterinary Internal Medicine, Seoul National University, 1 GwanakGwanak-ro, GwanakGwanak-gu, Seoul, Seoul 08840, Republic of Korea</t>
   </si>
   <si>
-    <t>PP334110, PP334109, PP334108, PP334107, PP334106, PP334105, PP334104, PP334103, PP334102, PP334101</t>
-  </si>
-  <si>
     <t>Sado yousseu F.</t>
   </si>
   <si>
@@ -203,16 +176,10 @@
     <t xml:space="preserve"> Faculty of Life Science and Technology, Kunming University of Science and Technology, 727 Jingming South Road, Kunming, Yunnan 650000, China</t>
   </si>
   <si>
-    <t>OQ633004, OQ633003, OQ633002</t>
-  </si>
-  <si>
     <t>Zhang Y., Sun S., Meng W., Muhetar R., Wang X., Ma J., Zhang F., Hu J., Dai X., Feng C., Hang C., Azati R., Tai X.</t>
   </si>
   <si>
     <t xml:space="preserve"> Xinjiang Center for Disease Control and Prevention, Key Lab of Biological Resources and Genetic Engineering of Xinjiang, College of Life Science and Technology, Xinjiang University 830046, P.R. China</t>
-  </si>
-  <si>
-    <t>DQ301505, DQ301504, DQ301503, DQ301502</t>
   </si>
   <si>
     <t>Genotypes of the congo-crimean hemorrhagic fever virus occurring in the turkestan region</t>
@@ -1434,6 +1401,39 @@
   </si>
   <si>
     <t>Parker M., Glass P., Jennings G., Lofts R., Smith J., Miller M., Glass P., Jennings G., Lofts R., Smith J., Miller M., Spik K., Schoepp R.</t>
+  </si>
+  <si>
+    <t>KT266832, KT266833, KT266834, KT266835, KT266836, KT266837, KT266838, KT266839, KT266840, KT266841, KT266842, KT266843, KT266844, KT266845, KT266846, KT266847, KT266848</t>
+  </si>
+  <si>
+    <t>PP449382, PP449383, PP449384, PP449385, PP449386</t>
+  </si>
+  <si>
+    <t>MW058028, MW058029, MW058030</t>
+  </si>
+  <si>
+    <t>ON500500, ON500501, ON500502</t>
+  </si>
+  <si>
+    <t>PP116318, PP116319, PP116320</t>
+  </si>
+  <si>
+    <t>MN689739, MN689740, MN689741</t>
+  </si>
+  <si>
+    <t>PP067047, PP067048, PP067049, PP067050, PP067051, PP067052, PP067053, PP067054, PP067055, PP067056, PP067057, PP067058, PP067059, PP067060, PP067061, PP067062, PP067063, PP067064, PP067065, PP067066, PP067067, PP067068, PP067069, PP067070, PP067071, PP067072, PP067073, PP067074, PP067075, PP067076, PP067077, PP067078, PP067079, PP067080, PP067081, PP067082, PP067083, PP067084, PP067085, PP067086, PP067087, PP067088</t>
+  </si>
+  <si>
+    <t>PP025038, PP025039, PP025040</t>
+  </si>
+  <si>
+    <t>PP334101, PP334102, PP334103, PP334104, PP334105, PP334106, PP334107, PP334108, PP334109, PP334110</t>
+  </si>
+  <si>
+    <t>OQ633002, OQ633003, OQ633004</t>
+  </si>
+  <si>
+    <t>DQ301502, DQ301503, DQ301504, DQ301505</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1841,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C81"/>
+      <selection activeCell="F2" sqref="F2:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1874,2165 +1874,2169 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>366</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E2" t="s">
-        <v>188</v>
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>2015</v>
       </c>
       <c r="F2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G2" s="5"/>
+        <v>417</v>
+      </c>
+      <c r="G2" s="6"/>
       <c r="H2" t="s">
-        <v>348</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>367</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" t="s">
-        <v>188</v>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>2024</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>418</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>328</v>
+        <v>269</v>
       </c>
       <c r="I3" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>116</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>368</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" t="s">
-        <v>150</v>
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
       </c>
       <c r="F4" t="s">
-        <v>151</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" t="s">
-        <v>317</v>
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>369</v>
-      </c>
-      <c r="D5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" t="s">
-        <v>192</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="G5" s="6"/>
       <c r="H5" t="s">
-        <v>329</v>
+        <v>270</v>
       </c>
       <c r="I5" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>370</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
-      </c>
-      <c r="E6" t="s">
-        <v>269</v>
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
       </c>
       <c r="F6" t="s">
-        <v>270</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>419</v>
+      </c>
+      <c r="G6" s="5">
+        <v>33416494</v>
+      </c>
       <c r="H6" t="s">
-        <v>353</v>
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>186</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>371</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" t="s">
-        <v>248</v>
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
       </c>
       <c r="F7" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>419</v>
+      </c>
+      <c r="G7" s="5">
+        <v>33416494</v>
+      </c>
       <c r="H7" t="s">
-        <v>347</v>
+        <v>271</v>
       </c>
       <c r="I7" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>2005</v>
+        <v>2022</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>420</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>372</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>2024</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>421</v>
+      </c>
+      <c r="G9" s="6"/>
       <c r="H9" t="s">
-        <v>310</v>
-      </c>
-      <c r="I9" t="s">
-        <v>355</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>373</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>235</v>
-      </c>
-      <c r="E10" t="s">
-        <v>236</v>
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>2019</v>
       </c>
       <c r="F10" t="s">
-        <v>237</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>422</v>
+      </c>
+      <c r="G10" s="5">
+        <v>33754998</v>
+      </c>
       <c r="H10" t="s">
-        <v>343</v>
+        <v>274</v>
+      </c>
+      <c r="I10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>374</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" t="s">
-        <v>177</v>
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>2023</v>
       </c>
       <c r="F11" t="s">
-        <v>178</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>423</v>
+      </c>
+      <c r="G11" s="6"/>
       <c r="H11" t="s">
-        <v>325</v>
-      </c>
-      <c r="I11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>375</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" t="s">
-        <v>108</v>
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>2023</v>
       </c>
       <c r="F12" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" s="5">
-        <v>19553586</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="G12" s="6"/>
       <c r="H12" t="s">
-        <v>340</v>
-      </c>
-      <c r="I12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>376</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" t="s">
-        <v>108</v>
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>2013</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" s="5">
-        <v>19523314</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G13" s="6"/>
       <c r="H13" t="s">
-        <v>305</v>
-      </c>
-      <c r="I13" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14">
+        <v>2024</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>425</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" t="s">
-        <v>281</v>
-      </c>
-      <c r="I14" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>377</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
-        <v>105</v>
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>2022</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="5">
-        <v>22119389</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="H15" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E16" t="s">
-        <v>218</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" t="s">
-        <v>337</v>
+        <v>280</v>
+      </c>
+      <c r="I16" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>379</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" t="s">
-        <v>139</v>
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>2023</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>362</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="G17" s="5"/>
       <c r="H17" t="s">
-        <v>314</v>
-      </c>
-      <c r="I17" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>380</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>213</v>
-      </c>
-      <c r="E18" t="s">
-        <v>214</v>
+        <v>47</v>
+      </c>
+      <c r="E18">
+        <v>2005</v>
       </c>
       <c r="F18" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>356</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="G18" s="6"/>
       <c r="H18" t="s">
-        <v>336</v>
-      </c>
-      <c r="I18" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" t="s">
-        <v>327</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>408</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20">
-        <v>2013</v>
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="G20" s="5">
+        <v>38446223</v>
+      </c>
       <c r="H20" t="s">
-        <v>288</v>
+        <v>284</v>
+      </c>
+      <c r="I20" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>190</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="D21" t="s">
-        <v>257</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>258</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>259</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>357</v>
+        <v>59</v>
+      </c>
+      <c r="G21" s="5">
+        <v>33388553</v>
       </c>
       <c r="H21" t="s">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="I21" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="H22" t="s">
-        <v>306</v>
+        <v>65</v>
       </c>
       <c r="I22" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="5">
-        <v>25108534</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G23" s="6"/>
       <c r="H23" t="s">
-        <v>313</v>
-      </c>
-      <c r="I23" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>173</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
         <v>385</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>234</v>
+        <v>72</v>
       </c>
       <c r="G24" s="5">
-        <v>33954213</v>
+        <v>31022170</v>
       </c>
       <c r="H24" t="s">
-        <v>342</v>
+        <v>286</v>
       </c>
       <c r="I24" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>191</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>260</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="D25" t="s">
-        <v>261</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>262</v>
+        <v>67</v>
       </c>
       <c r="F25" t="s">
-        <v>263</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="G25" s="5">
+        <v>34662872</v>
+      </c>
       <c r="H25" t="s">
-        <v>351</v>
+        <v>287</v>
       </c>
       <c r="I25" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>387</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>2015</v>
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>184</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>243</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>387</v>
+        <v>409</v>
       </c>
       <c r="D27" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>245</v>
+        <v>54</v>
       </c>
       <c r="F27" t="s">
-        <v>246</v>
+        <v>80</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>365</v>
+        <v>267</v>
       </c>
       <c r="H27" t="s">
-        <v>346</v>
+        <v>289</v>
       </c>
       <c r="I27" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
       <c r="F28" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
       <c r="G28" s="5">
-        <v>27523802</v>
+        <v>39565134</v>
       </c>
       <c r="H28" t="s">
-        <v>332</v>
+        <v>290</v>
+      </c>
+      <c r="I28" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D29" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="G29" s="5">
+        <v>31291242</v>
+      </c>
       <c r="H29" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="I29" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>239</v>
-      </c>
-      <c r="G30" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="G30" s="5">
+        <v>27926935</v>
+      </c>
       <c r="H30" t="s">
-        <v>344</v>
+        <v>292</v>
+      </c>
+      <c r="I30" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G31" s="5">
-        <v>27926935</v>
+        <v>22119389</v>
       </c>
       <c r="H31" t="s">
-        <v>303</v>
-      </c>
-      <c r="I31" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G32" s="5">
-        <v>28251517</v>
+        <v>19523314</v>
       </c>
       <c r="H32" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="I32" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>194</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>196</v>
-      </c>
-      <c r="G33" s="5">
-        <v>29148370</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G33" s="5"/>
       <c r="H33" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="I33" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
         <v>394</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
       <c r="F34" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="G34" s="5">
-        <v>28902913</v>
+        <v>33142046</v>
       </c>
       <c r="H34" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="I34" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>197</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="D35" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>199</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>363</v>
+        <v>107</v>
+      </c>
+      <c r="G35" s="5">
+        <v>28251517</v>
       </c>
       <c r="H35" t="s">
-        <v>331</v>
+        <v>297</v>
+      </c>
+      <c r="I35" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="5">
-        <v>31022170</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="G36" s="5"/>
       <c r="H36" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I36" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="D37" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="E37" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
-        <v>164</v>
-      </c>
-      <c r="G37" s="5">
-        <v>31107219</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="G37" s="5"/>
       <c r="H37" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="I37" t="s">
-        <v>277</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>398</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
-      </c>
-      <c r="G38" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="G38" s="5"/>
       <c r="H38" t="s">
-        <v>299</v>
+        <v>300</v>
+      </c>
+      <c r="I38" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>240</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>119</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>242</v>
-      </c>
-      <c r="G39" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="G39" s="5">
+        <v>28902913</v>
+      </c>
       <c r="H39" t="s">
-        <v>345</v>
+        <v>301</v>
       </c>
       <c r="I39" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C40" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="G40" s="5">
-        <v>31211933</v>
+        <v>25108534</v>
       </c>
       <c r="H40" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="I40" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="C41" t="s">
-        <v>401</v>
+        <v>368</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="E41" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
-      </c>
-      <c r="G41" s="5">
-        <v>32738065</v>
+        <v>129</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>351</v>
       </c>
       <c r="H41" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="I41" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="s">
+        <v>389</v>
+      </c>
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
         <v>71</v>
       </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" t="s">
-        <v>402</v>
-      </c>
-      <c r="D42" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" t="s">
-        <v>69</v>
-      </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="G42" s="5">
-        <v>31291242</v>
+        <v>31211933</v>
       </c>
       <c r="H42" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="I42" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
       <c r="D43" t="s">
-        <v>207</v>
+        <v>134</v>
       </c>
       <c r="E43" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="F43" t="s">
-        <v>208</v>
-      </c>
-      <c r="G43" s="5">
-        <v>35551538</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="G43" s="5"/>
       <c r="H43" t="s">
-        <v>334</v>
-      </c>
-      <c r="I43" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>357</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44">
-        <v>2019</v>
+        <v>138</v>
+      </c>
+      <c r="E44" t="s">
+        <v>139</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>141</v>
       </c>
       <c r="C45" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F45" t="s">
-        <v>206</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>364</v>
+        <v>143</v>
+      </c>
+      <c r="G45" s="5">
+        <v>40045205</v>
       </c>
       <c r="H45" t="s">
-        <v>333</v>
+        <v>307</v>
+      </c>
+      <c r="I45" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="F46" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="G46" s="5">
-        <v>33142046</v>
+        <v>32738065</v>
       </c>
       <c r="H46" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I46" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="C47" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F47" t="s">
-        <v>70</v>
-      </c>
-      <c r="G47" s="5">
-        <v>33388553</v>
+        <v>150</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="H47" t="s">
-        <v>71</v>
+        <v>309</v>
       </c>
       <c r="I47" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>386</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48">
-        <v>2019</v>
+        <v>152</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
       </c>
       <c r="F48" t="s">
-        <v>35</v>
+        <v>153</v>
       </c>
       <c r="G48" s="5">
-        <v>33754998</v>
+        <v>31107219</v>
       </c>
       <c r="H48" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="I48" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>396</v>
+      </c>
+      <c r="D49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" t="s">
+        <v>156</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
-      </c>
-      <c r="G49" s="5"/>
+        <v>157</v>
+      </c>
+      <c r="G49" s="5">
+        <v>33421655</v>
+      </c>
       <c r="H49" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="I49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>126</v>
+        <v>412</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="E50" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F50" t="s">
-        <v>128</v>
-      </c>
-      <c r="G50" s="5"/>
+        <v>160</v>
+      </c>
+      <c r="G50" s="5">
+        <v>39238565</v>
+      </c>
       <c r="H50" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I50" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C51" t="s">
         <v>407</v>
       </c>
       <c r="D51" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E51" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
       <c r="F51" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G51" s="5">
-        <v>33421655</v>
+        <v>37766297</v>
       </c>
       <c r="H51" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="I51" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>188</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>253</v>
+        <v>164</v>
       </c>
       <c r="C52" t="s">
-        <v>408</v>
+        <v>363</v>
       </c>
       <c r="D52" t="s">
-        <v>254</v>
+        <v>165</v>
       </c>
       <c r="E52" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" t="s">
         <v>167</v>
       </c>
-      <c r="F52" t="s">
-        <v>255</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>275</v>
-      </c>
+      <c r="G52" s="5"/>
       <c r="H52" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="I52" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>416</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53">
-        <v>2021</v>
+        <v>168</v>
+      </c>
+      <c r="E53" t="s">
+        <v>169</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
-      </c>
-      <c r="G53" s="5">
-        <v>33416494</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="G53" s="6"/>
       <c r="H53" t="s">
-        <v>24</v>
-      </c>
-      <c r="I53" t="s">
-        <v>277</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>370</v>
       </c>
       <c r="D54" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54">
-        <v>2020</v>
+        <v>172</v>
+      </c>
+      <c r="E54" t="s">
+        <v>173</v>
       </c>
       <c r="F54" t="s">
-        <v>23</v>
-      </c>
-      <c r="G54" s="5">
-        <v>33416494</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G54" s="5"/>
       <c r="H54" t="s">
-        <v>282</v>
-      </c>
-      <c r="I54" t="s">
-        <v>276</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="D55" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="F55" t="s">
-        <v>222</v>
-      </c>
-      <c r="G55" s="5">
-        <v>35531170</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="G55" s="6"/>
       <c r="H55" t="s">
-        <v>338</v>
+        <v>317</v>
+      </c>
+      <c r="I55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
       <c r="D56" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="E56" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="F56" t="s">
-        <v>211</v>
-      </c>
-      <c r="G56" s="5">
-        <v>33672497</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G56" s="5"/>
       <c r="H56" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="I56" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>184</v>
       </c>
       <c r="E57" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="F57" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="G57" s="5">
-        <v>34662872</v>
+        <v>29148370</v>
       </c>
       <c r="H57" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="I57" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>203</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
-        <v>412</v>
+        <v>384</v>
       </c>
       <c r="D58" t="s">
-        <v>271</v>
+        <v>187</v>
       </c>
       <c r="E58" t="s">
-        <v>272</v>
+        <v>71</v>
       </c>
       <c r="F58" t="s">
-        <v>273</v>
-      </c>
-      <c r="G58" s="5"/>
+        <v>188</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>352</v>
+      </c>
       <c r="H58" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>189</v>
       </c>
       <c r="C59" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
       <c r="D59" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>191</v>
       </c>
       <c r="F59" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" s="6"/>
+        <v>192</v>
+      </c>
+      <c r="G59" s="5">
+        <v>27523802</v>
+      </c>
       <c r="H59" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>393</v>
       </c>
       <c r="D60" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60">
-        <v>2022</v>
+        <v>194</v>
+      </c>
+      <c r="E60" t="s">
+        <v>58</v>
       </c>
       <c r="F60" t="s">
-        <v>29</v>
-      </c>
-      <c r="G60" s="6"/>
+        <v>195</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="H60" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
       <c r="D61" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61">
-        <v>2022</v>
+        <v>196</v>
+      </c>
+      <c r="E61" t="s">
+        <v>58</v>
       </c>
       <c r="F61" t="s">
-        <v>50</v>
-      </c>
-      <c r="G61" s="5"/>
+        <v>197</v>
+      </c>
+      <c r="G61" s="5">
+        <v>35551538</v>
+      </c>
       <c r="H61" t="s">
-        <v>290</v>
+        <v>323</v>
+      </c>
+      <c r="I61" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
-        <v>264</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D62" t="s">
-        <v>265</v>
+        <v>199</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F62" t="s">
+        <v>200</v>
+      </c>
+      <c r="G62" s="5">
+        <v>33672497</v>
+      </c>
+      <c r="H62" t="s">
+        <v>324</v>
+      </c>
+      <c r="I62" t="s">
         <v>266</v>
-      </c>
-      <c r="G62" s="5">
-        <v>37527191</v>
-      </c>
-      <c r="H62" t="s">
-        <v>352</v>
-      </c>
-      <c r="I62" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="C63" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>203</v>
       </c>
       <c r="F63" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>274</v>
+        <v>345</v>
       </c>
       <c r="H63" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="I63" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>205</v>
       </c>
       <c r="C64" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>207</v>
       </c>
       <c r="F64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>361</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="G64" s="5"/>
       <c r="H64" t="s">
-        <v>76</v>
-      </c>
-      <c r="I64" t="s">
-        <v>276</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>53</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>210</v>
       </c>
       <c r="F65" t="s">
-        <v>62</v>
-      </c>
-      <c r="G65" s="6"/>
+        <v>211</v>
+      </c>
+      <c r="G65" s="5">
+        <v>35531170</v>
+      </c>
       <c r="H65" t="s">
-        <v>294</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="C66" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="D66" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="E66" t="s">
-        <v>65</v>
+        <v>214</v>
       </c>
       <c r="F66" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="G66" s="5">
-        <v>37766297</v>
+        <v>37879367</v>
       </c>
       <c r="H66" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="I66" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>419</v>
+        <v>364</v>
       </c>
       <c r="D67" t="s">
-        <v>64</v>
+        <v>216</v>
       </c>
       <c r="E67" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="F67" t="s">
-        <v>66</v>
+        <v>217</v>
       </c>
       <c r="G67" s="5">
-        <v>38446223</v>
+        <v>19553586</v>
       </c>
       <c r="H67" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="I67" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="C68" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="D68" t="s">
-        <v>64</v>
+        <v>219</v>
       </c>
       <c r="E68" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F68" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>278</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="G68" s="6"/>
       <c r="H68" t="s">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="I68" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B69" t="s">
+        <v>221</v>
+      </c>
+      <c r="C69" t="s">
+        <v>374</v>
+      </c>
+      <c r="D69" t="s">
+        <v>222</v>
+      </c>
+      <c r="E69" t="s">
+        <v>191</v>
+      </c>
+      <c r="F69" t="s">
         <v>223</v>
       </c>
-      <c r="C69" t="s">
-        <v>421</v>
-      </c>
-      <c r="D69" t="s">
-        <v>224</v>
-      </c>
-      <c r="E69" t="s">
-        <v>225</v>
-      </c>
-      <c r="F69" t="s">
-        <v>226</v>
-      </c>
       <c r="G69" s="5">
-        <v>37879367</v>
+        <v>33954213</v>
       </c>
       <c r="H69" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="I69" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>362</v>
       </c>
       <c r="D70" t="s">
-        <v>54</v>
-      </c>
-      <c r="E70">
-        <v>2023</v>
+        <v>224</v>
+      </c>
+      <c r="E70" t="s">
+        <v>225</v>
       </c>
       <c r="F70" t="s">
-        <v>55</v>
+        <v>226</v>
       </c>
       <c r="G70" s="5"/>
       <c r="H70" t="s">
-        <v>292</v>
+        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
-        <v>152</v>
+        <v>227</v>
       </c>
       <c r="C71" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>70</v>
       </c>
       <c r="E71" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F71" t="s">
-        <v>154</v>
-      </c>
-      <c r="G71" s="5">
-        <v>40045205</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="G71" s="6"/>
       <c r="H71" t="s">
-        <v>318</v>
-      </c>
-      <c r="I71" t="s">
-        <v>277</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
-        <v>423</v>
+        <v>388</v>
       </c>
       <c r="D72" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="E72" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F72" t="s">
-        <v>171</v>
-      </c>
-      <c r="G72" s="5">
-        <v>39238565</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="G72" s="6"/>
       <c r="H72" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="I72" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>34</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>376</v>
       </c>
       <c r="D73" t="s">
-        <v>40</v>
-      </c>
-      <c r="E73">
-        <v>2023</v>
+        <v>233</v>
+      </c>
+      <c r="E73" t="s">
+        <v>234</v>
       </c>
       <c r="F73" t="s">
-        <v>41</v>
-      </c>
-      <c r="G73" s="6"/>
+        <v>235</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>354</v>
+      </c>
       <c r="H73" t="s">
-        <v>287</v>
+        <v>335</v>
+      </c>
+      <c r="I73" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>33</v>
+        <v>186</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>36</v>
+        <v>360</v>
       </c>
       <c r="D74" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74">
-        <v>2023</v>
+        <v>236</v>
+      </c>
+      <c r="E74" t="s">
+        <v>237</v>
       </c>
       <c r="F74" t="s">
-        <v>38</v>
+        <v>238</v>
       </c>
       <c r="G74" s="6"/>
       <c r="H74" t="s">
-        <v>286</v>
+        <v>336</v>
+      </c>
+      <c r="I74" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>239</v>
       </c>
       <c r="C75" t="s">
-        <v>30</v>
+        <v>355</v>
       </c>
       <c r="D75" t="s">
-        <v>31</v>
-      </c>
-      <c r="E75">
-        <v>2024</v>
+        <v>240</v>
+      </c>
+      <c r="E75" t="s">
+        <v>177</v>
       </c>
       <c r="F75" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="6"/>
+        <v>241</v>
+      </c>
+      <c r="G75" s="5"/>
       <c r="H75" t="s">
-        <v>284</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>36</v>
+        <v>188</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>397</v>
       </c>
       <c r="D76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E76">
-        <v>2024</v>
+        <v>243</v>
+      </c>
+      <c r="E76" t="s">
+        <v>156</v>
       </c>
       <c r="F76" t="s">
-        <v>47</v>
-      </c>
-      <c r="G76" s="6"/>
+        <v>244</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>264</v>
+      </c>
       <c r="H76" t="s">
-        <v>289</v>
+        <v>338</v>
+      </c>
+      <c r="I76" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>3</v>
+        <v>190</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>245</v>
       </c>
       <c r="C77" t="s">
-        <v>10</v>
+        <v>371</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77">
-        <v>2024</v>
+        <v>246</v>
+      </c>
+      <c r="E77" t="s">
+        <v>247</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="6"/>
+        <v>248</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>346</v>
+      </c>
       <c r="H77" t="s">
-        <v>280</v>
+        <v>339</v>
       </c>
       <c r="I77" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B78" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="C78" t="s">
-        <v>424</v>
+        <v>375</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="E78" t="s">
-        <v>94</v>
+        <v>251</v>
       </c>
       <c r="F78" t="s">
-        <v>231</v>
-      </c>
-      <c r="G78" s="6"/>
+        <v>252</v>
+      </c>
+      <c r="G78" s="5"/>
       <c r="H78" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I78" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="C79" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="D79" t="s">
-        <v>93</v>
+        <v>254</v>
       </c>
       <c r="E79" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="G79" s="5">
-        <v>39565134</v>
+        <v>37527191</v>
       </c>
       <c r="H79" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="I79" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="B80" t="s">
-        <v>144</v>
+        <v>256</v>
       </c>
       <c r="C80" t="s">
-        <v>426</v>
+        <v>359</v>
       </c>
       <c r="D80" t="s">
-        <v>145</v>
+        <v>257</v>
       </c>
       <c r="E80" t="s">
-        <v>146</v>
+        <v>258</v>
       </c>
       <c r="F80" t="s">
-        <v>147</v>
-      </c>
-      <c r="G80" s="5"/>
+        <v>259</v>
+      </c>
+      <c r="G80" s="6"/>
       <c r="H80" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="D81" t="s">
-        <v>179</v>
+        <v>260</v>
       </c>
       <c r="E81" t="s">
-        <v>180</v>
+        <v>261</v>
       </c>
       <c r="F81" t="s">
-        <v>181</v>
-      </c>
-      <c r="G81" s="6"/>
+        <v>262</v>
+      </c>
+      <c r="G81" s="5"/>
       <c r="H81" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I81" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I81">
+      <sortCondition ref="A1:A81"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
remove mouse model accessions
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392F8A22-FB7F-B54F-B5F1-DF004DCB8D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76564A0-A35A-C149-851F-183AD2A81540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="500" windowWidth="25740" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11500" yWindow="500" windowWidth="32160" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="419">
   <si>
     <t>RefID</t>
   </si>
@@ -90,24 +90,6 @@
   </si>
   <si>
     <t>FJ472634</t>
-  </si>
-  <si>
-    <t>Immunocompetent Mouse Model for Crimean-Congo Hemorrhagic Fever Virus</t>
-  </si>
-  <si>
-    <t>Hawman D., Meade-white K., Leventhal S., Feldmann F., Okumura A., Smith B., Scott D., Feldmann H.</t>
-  </si>
-  <si>
-    <t>bioRxiv (2021) In press</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The publication associated with the GenBank accessions MW058030, MW058029, and MW058028 is titled "Immunocompetent Mouse Model for Crimean-Congo Hemorrhagic Fever Virus" by authors David W. Hawman, Kimberly Meade-White, Shanna Leventhal, Friederike Feldmann, Atsushi Okumura, Brian Smith, Dana Scott, and Heinz Feldmann. It was published in *eLife* on January 8, 2021. The PubMed ID (PMID) for this article is 33416494. ([pubmed.ncbi.nlm.nih.gov](https://pubmed.ncbi.nlm.nih.gov/33416494/?utm_source=openai)) </t>
-  </si>
-  <si>
-    <t>Hawman D., Sturdevant D., Martens C., Babian K., Feldmann H.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laboratory of Virology, Rocky Mountain Labs NIH/NIAD, 903 S 4th St, Hamilton, MT 59840, USA</t>
   </si>
   <si>
     <t>Ji J., Zhou H., Cui M., Guo M., Ma Z., Li L., Hu T., Shi W.</t>
@@ -857,9 +839,6 @@
   </si>
   <si>
     <t xml:space="preserve">The publication associated with the GenBank accession number FJ472634 is titled "Crimean-Congo Hemorrhagic Fever, Southwestern Bulgaria," authored by Christova I., Di Caro A., Papa A., Castilletti C., Andonova L., Kalvatchev N., Papadimitriou E., Carletti F., Mohareb E., Capobianchi M.R., Ippolito G., and Rezza G. It was published in the journal *Emerging Infectious Diseases* in June 2009 (Volume 15, Issue 6, pages 983–985). The article is available at https://wwwnc.cdc.gov/eid/article/15/6/08-1567_article. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The GenBank submissions with accession numbers MW058030, MW058029, and MW058028 are associated with the study titled "A DNA-based vaccine protects against Crimean-Congo haemorrhagic fever virus disease in a Cynomolgus macaque model," authored by David W. Hawman, Kimberly Meade-White, Patrick W. Hanley, Dana Scott, Atsushi Okumura, Heinz Feldmann, Gustaf Ahlén, K. Sofia Appelberg, Vanessa Monteil, Stephanie Devignot, Friedemann Weber, Matti Sällberg, and Ali Mirazimi. This study was published in *Nature Microbiology* in 2021. The DOI for this publication is 10.1038/s41564-020-00815-6. ([nature.com](https://www.nature.com/articles/s41564-020-00815-6?utm_source=openai)) </t>
   </si>
   <si>
     <t xml:space="preserve">I searched for publications associated with the GenBank submissions ON500502, ON500501, and ON500500, authored by Ji J., Zhou H., Cui M., Guo M., Ma Z., Li L., Hu T., and Shi W. from the Key Laboratory of Etiology and Epidemiology of Emerging Infectious Diseases, Shandong First Medical University and Shandong Academy of Medical Sciences, Taian, China, in 2022. Unfortunately, I couldn't locate a corresponding publication in PubMed or other bibliographic databases. It's possible that the study related to these GenBank entries hasn't been published yet or isn't indexed in the databases I searched. </t>
@@ -1187,9 +1166,6 @@
     <t>no, retrive from GenBank</t>
   </si>
   <si>
-    <t>23195573, 22616022</t>
-  </si>
-  <si>
     <t>10.3103/S0891416814040132, 25845138</t>
   </si>
   <si>
@@ -1407,9 +1383,6 @@
   </si>
   <si>
     <t>PP449382, PP449383, PP449384, PP449385, PP449386</t>
-  </si>
-  <si>
-    <t>MW058028, MW058029, MW058030</t>
   </si>
   <si>
     <t>ON500500, ON500501, ON500502</t>
@@ -1838,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F81"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1874,13 +1847,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1900,11 +1873,11 @@
         <v>2015</v>
       </c>
       <c r="F2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1924,14 +1897,14 @@
         <v>2024</v>
       </c>
       <c r="F3" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1958,7 +1931,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1976,678 +1949,675 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F6" t="s">
-        <v>419</v>
-      </c>
-      <c r="G6" s="5">
-        <v>33416494</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
-      </c>
-      <c r="G7" s="5">
-        <v>33416494</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="H7" t="s">
-        <v>271</v>
-      </c>
-      <c r="I7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="F8" t="s">
-        <v>420</v>
-      </c>
-      <c r="G8" s="6"/>
+        <v>413</v>
+      </c>
+      <c r="G8" s="5">
+        <v>33754998</v>
+      </c>
       <c r="H8" t="s">
-        <v>272</v>
+        <v>267</v>
+      </c>
+      <c r="I8" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="F9" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="F10" t="s">
-        <v>422</v>
-      </c>
-      <c r="G10" s="5">
-        <v>33754998</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="G10" s="6"/>
       <c r="H10" t="s">
-        <v>274</v>
-      </c>
-      <c r="I10" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>2013</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <v>2023</v>
-      </c>
-      <c r="F11" t="s">
-        <v>423</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
       <c r="E12">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F12" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13">
+        <v>2022</v>
+      </c>
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="E13">
-        <v>2013</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="5"/>
       <c r="H13" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14">
-        <v>2024</v>
-      </c>
       <c r="F14" t="s">
-        <v>425</v>
-      </c>
-      <c r="G14" s="6"/>
+        <v>413</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14" t="s">
-        <v>278</v>
+        <v>273</v>
+      </c>
+      <c r="I14" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>40</v>
-      </c>
       <c r="E15">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>417</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16">
+        <v>2005</v>
       </c>
       <c r="F16" t="s">
-        <v>422</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>418</v>
+      </c>
+      <c r="G16" s="6"/>
       <c r="H16" t="s">
-        <v>280</v>
-      </c>
-      <c r="I16" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
+        <v>398</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>45</v>
       </c>
-      <c r="E17">
-        <v>2023</v>
-      </c>
-      <c r="F17" t="s">
-        <v>426</v>
-      </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="6"/>
       <c r="H17" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>400</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
-      <c r="E18">
-        <v>2005</v>
+      <c r="E18" t="s">
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>427</v>
-      </c>
-      <c r="G18" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="G18" s="5">
+        <v>38446223</v>
+      </c>
       <c r="H18" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="I18" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>387</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>406</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="5">
+        <v>33388553</v>
+      </c>
       <c r="H19" t="s">
-        <v>283</v>
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="5">
-        <v>38446223</v>
+        <v>58</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="H20" t="s">
-        <v>284</v>
+        <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="5">
-        <v>33388553</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G21" s="6"/>
       <c r="H21" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>405</v>
+        <v>377</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>350</v>
+        <v>66</v>
+      </c>
+      <c r="G22" s="5">
+        <v>31022170</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>279</v>
       </c>
       <c r="I22" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="G23" s="5">
+        <v>34662872</v>
+      </c>
       <c r="H23" t="s">
-        <v>285</v>
+        <v>280</v>
+      </c>
+      <c r="I23" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
         <v>72</v>
       </c>
-      <c r="G24" s="5">
-        <v>31022170</v>
-      </c>
+      <c r="G24" s="6"/>
       <c r="H24" t="s">
-        <v>286</v>
-      </c>
-      <c r="I24" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
         <v>74</v>
       </c>
-      <c r="E25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="5">
-        <v>34662872</v>
+      <c r="G25" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="H25" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I25" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>406</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
-        <v>387</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>77</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
       </c>
       <c r="F26" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="6"/>
+      <c r="G26" s="5">
+        <v>39565134</v>
+      </c>
       <c r="H26" t="s">
-        <v>288</v>
+        <v>283</v>
+      </c>
+      <c r="I26" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>267</v>
+        <v>81</v>
+      </c>
+      <c r="G27" s="5">
+        <v>31291242</v>
       </c>
       <c r="H27" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I27" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>414</v>
+        <v>372</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G28" s="5">
-        <v>39565134</v>
+        <v>27926935</v>
       </c>
       <c r="H28" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I28" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>391</v>
+        <v>358</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G29" s="5">
-        <v>31291242</v>
+        <v>22119389</v>
       </c>
       <c r="H29" t="s">
-        <v>291</v>
-      </c>
-      <c r="I29" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G30" s="5">
-        <v>27926935</v>
+        <v>19523314</v>
       </c>
       <c r="H30" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I30" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D31" t="s">
         <v>93</v>
@@ -2658,1385 +2628,1326 @@
       <c r="F31" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="5">
-        <v>22119389</v>
-      </c>
+      <c r="G31" s="5"/>
       <c r="H31" t="s">
-        <v>293</v>
+        <v>288</v>
+      </c>
+      <c r="I31" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
         <v>98</v>
       </c>
       <c r="G32" s="5">
-        <v>19523314</v>
+        <v>33142046</v>
       </c>
       <c r="H32" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I32" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F33" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5">
+        <v>28251517</v>
+      </c>
       <c r="H33" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I33" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
         <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="D34" t="s">
         <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="F34" t="s">
         <v>104</v>
       </c>
-      <c r="G34" s="5">
-        <v>33142046</v>
-      </c>
+      <c r="G34" s="5"/>
       <c r="H34" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I34" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
         <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
       <c r="D35" t="s">
         <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="5">
-        <v>28251517</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G35" s="5"/>
       <c r="H35" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I35" t="s">
-        <v>266</v>
+        <v>337</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>378</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I36" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G37" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="G37" s="5">
+        <v>28902913</v>
+      </c>
       <c r="H37" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I37" t="s">
-        <v>344</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>365</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>117</v>
-      </c>
-      <c r="G38" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="G38" s="5">
+        <v>25108534</v>
+      </c>
       <c r="H38" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I38" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E39" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="5">
-        <v>28902913</v>
+        <v>123</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="H39" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I39" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G40" s="5">
-        <v>25108534</v>
+        <v>31211933</v>
       </c>
       <c r="H40" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I40" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C41" t="s">
-        <v>368</v>
+        <v>407</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F41" t="s">
-        <v>129</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>351</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G41" s="5"/>
       <c r="H41" t="s">
-        <v>303</v>
-      </c>
-      <c r="I41" t="s">
-        <v>265</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="F42" t="s">
-        <v>132</v>
-      </c>
-      <c r="G42" s="5">
-        <v>31211933</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G42" s="5"/>
       <c r="H42" t="s">
-        <v>304</v>
-      </c>
-      <c r="I42" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="F43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G43" s="5"/>
+        <v>137</v>
+      </c>
+      <c r="G43" s="5">
+        <v>40045205</v>
+      </c>
       <c r="H43" t="s">
-        <v>305</v>
+        <v>300</v>
+      </c>
+      <c r="I43" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C44" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F44" t="s">
-        <v>140</v>
-      </c>
-      <c r="G44" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="G44" s="5">
+        <v>32738065</v>
+      </c>
       <c r="H44" t="s">
-        <v>306</v>
+        <v>301</v>
+      </c>
+      <c r="I44" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C45" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" s="5">
-        <v>40045205</v>
+        <v>144</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="H45" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I45" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F46" t="s">
         <v>147</v>
       </c>
       <c r="G46" s="5">
-        <v>32738065</v>
+        <v>31107219</v>
       </c>
       <c r="H46" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="I46" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B47" t="s">
         <v>148</v>
       </c>
       <c r="C47" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D47" t="s">
         <v>149</v>
       </c>
       <c r="E47" t="s">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="F47" t="s">
-        <v>150</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>263</v>
+        <v>151</v>
+      </c>
+      <c r="G47" s="5">
+        <v>33421655</v>
       </c>
       <c r="H47" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I47" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C48" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="F48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G48" s="5">
-        <v>31107219</v>
+        <v>39238565</v>
       </c>
       <c r="H48" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I48" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
+        <v>48</v>
       </c>
       <c r="F49" t="s">
         <v>157</v>
       </c>
       <c r="G49" s="5">
-        <v>33421655</v>
+        <v>37766297</v>
       </c>
       <c r="H49" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I49" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
         <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>412</v>
+        <v>355</v>
       </c>
       <c r="D50" t="s">
         <v>159</v>
       </c>
       <c r="E50" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="F50" t="s">
-        <v>160</v>
-      </c>
-      <c r="G50" s="5">
-        <v>39238565</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G50" s="5"/>
       <c r="H50" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I50" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D51" t="s">
         <v>162</v>
       </c>
       <c r="E51" t="s">
-        <v>54</v>
+        <v>163</v>
       </c>
       <c r="F51" t="s">
-        <v>163</v>
-      </c>
-      <c r="G51" s="5">
-        <v>37766297</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="G51" s="6"/>
       <c r="H51" t="s">
-        <v>313</v>
-      </c>
-      <c r="I51" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F52" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" t="s">
-        <v>314</v>
-      </c>
-      <c r="I52" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>416</v>
+        <v>348</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E53" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F53" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G53" s="6"/>
       <c r="H53" t="s">
-        <v>315</v>
+        <v>310</v>
+      </c>
+      <c r="I53" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F54" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" t="s">
-        <v>316</v>
+        <v>311</v>
+      </c>
+      <c r="I54" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C55" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="D55" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>114</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
-      </c>
-      <c r="G55" s="6"/>
+        <v>179</v>
+      </c>
+      <c r="G55" s="5">
+        <v>29148370</v>
+      </c>
       <c r="H55" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I55" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E56" t="s">
-        <v>181</v>
+        <v>65</v>
       </c>
       <c r="F56" t="s">
         <v>182</v>
       </c>
-      <c r="G56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>344</v>
+      </c>
       <c r="H56" t="s">
-        <v>318</v>
-      </c>
-      <c r="I56" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
         <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="D57" t="s">
         <v>184</v>
       </c>
       <c r="E57" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="F57" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G57" s="5">
-        <v>29148370</v>
+        <v>27523802</v>
       </c>
       <c r="H57" t="s">
-        <v>319</v>
-      </c>
-      <c r="I57" t="s">
-        <v>266</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H58" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D59" t="s">
         <v>190</v>
       </c>
       <c r="E59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" t="s">
         <v>191</v>
       </c>
-      <c r="F59" t="s">
-        <v>192</v>
-      </c>
       <c r="G59" s="5">
-        <v>27523802</v>
+        <v>35551538</v>
       </c>
       <c r="H59" t="s">
-        <v>321</v>
+        <v>316</v>
+      </c>
+      <c r="I59" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" t="s">
+        <v>391</v>
+      </c>
+      <c r="D60" t="s">
         <v>193</v>
       </c>
-      <c r="C60" t="s">
-        <v>393</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F60" t="s">
         <v>194</v>
       </c>
-      <c r="E60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F60" t="s">
-        <v>195</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>353</v>
+      <c r="G60" s="5">
+        <v>33672497</v>
       </c>
       <c r="H60" t="s">
-        <v>322</v>
+        <v>317</v>
+      </c>
+      <c r="I60" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="D61" t="s">
         <v>196</v>
       </c>
       <c r="E61" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="F61" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G61" s="5">
-        <v>35551538</v>
+        <v>23195573</v>
       </c>
       <c r="H61" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I61" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C62" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="D62" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E62" t="s">
-        <v>67</v>
+        <v>201</v>
       </c>
       <c r="F62" t="s">
-        <v>200</v>
-      </c>
-      <c r="G62" s="5">
-        <v>33672497</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="G62" s="5"/>
       <c r="H62" t="s">
-        <v>324</v>
-      </c>
-      <c r="I62" t="s">
-        <v>266</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B63" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E63" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F63" t="s">
-        <v>204</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>345</v>
+        <v>205</v>
+      </c>
+      <c r="G63" s="5">
+        <v>35531170</v>
       </c>
       <c r="H63" t="s">
-        <v>325</v>
-      </c>
-      <c r="I63" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
       <c r="D64" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E64" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F64" t="s">
-        <v>208</v>
-      </c>
-      <c r="G64" s="5"/>
+        <v>209</v>
+      </c>
+      <c r="G64" s="5">
+        <v>37879367</v>
+      </c>
       <c r="H64" t="s">
-        <v>326</v>
+        <v>321</v>
+      </c>
+      <c r="I64" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>398</v>
+        <v>356</v>
       </c>
       <c r="D65" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E65" t="s">
-        <v>210</v>
+        <v>91</v>
       </c>
       <c r="F65" t="s">
         <v>211</v>
       </c>
       <c r="G65" s="5">
-        <v>35531170</v>
+        <v>19553586</v>
       </c>
       <c r="H65" t="s">
-        <v>327</v>
+        <v>322</v>
+      </c>
+      <c r="I65" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
         <v>212</v>
       </c>
       <c r="C66" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D66" t="s">
         <v>213</v>
       </c>
       <c r="E66" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" t="s">
         <v>214</v>
       </c>
-      <c r="F66" t="s">
-        <v>215</v>
-      </c>
-      <c r="G66" s="5">
-        <v>37879367</v>
-      </c>
+      <c r="G66" s="6"/>
       <c r="H66" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I66" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>215</v>
       </c>
       <c r="C67" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D67" t="s">
         <v>216</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="F67" t="s">
         <v>217</v>
       </c>
       <c r="G67" s="5">
-        <v>19553586</v>
+        <v>33954213</v>
       </c>
       <c r="H67" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I67" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>354</v>
+      </c>
+      <c r="D68" t="s">
         <v>218</v>
       </c>
-      <c r="C68" t="s">
-        <v>413</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>219</v>
-      </c>
-      <c r="E68" t="s">
-        <v>83</v>
       </c>
       <c r="F68" t="s">
         <v>220</v>
       </c>
-      <c r="G68" s="6"/>
+      <c r="G68" s="5"/>
       <c r="H68" t="s">
-        <v>330</v>
-      </c>
-      <c r="I68" t="s">
-        <v>265</v>
+        <v>325</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B69" t="s">
         <v>221</v>
       </c>
       <c r="C69" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" t="s">
         <v>222</v>
       </c>
-      <c r="E69" t="s">
-        <v>191</v>
-      </c>
-      <c r="F69" t="s">
-        <v>223</v>
-      </c>
-      <c r="G69" s="5">
-        <v>33954213</v>
-      </c>
+      <c r="G69" s="6"/>
       <c r="H69" t="s">
-        <v>331</v>
-      </c>
-      <c r="I69" t="s">
-        <v>266</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>223</v>
       </c>
       <c r="C70" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="D70" t="s">
         <v>224</v>
       </c>
       <c r="E70" t="s">
+        <v>65</v>
+      </c>
+      <c r="F70" t="s">
         <v>225</v>
       </c>
-      <c r="F70" t="s">
-        <v>226</v>
-      </c>
-      <c r="G70" s="5"/>
+      <c r="G70" s="6"/>
       <c r="H70" t="s">
-        <v>332</v>
+        <v>327</v>
+      </c>
+      <c r="I70" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B71" t="s">
+        <v>226</v>
+      </c>
+      <c r="C71" t="s">
+        <v>368</v>
+      </c>
+      <c r="D71" t="s">
         <v>227</v>
       </c>
-      <c r="C71" t="s">
-        <v>379</v>
-      </c>
-      <c r="D71" t="s">
-        <v>70</v>
-      </c>
       <c r="E71" t="s">
-        <v>90</v>
+        <v>228</v>
       </c>
       <c r="F71" t="s">
-        <v>228</v>
-      </c>
-      <c r="G71" s="6"/>
+        <v>229</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>346</v>
+      </c>
       <c r="H71" t="s">
-        <v>333</v>
+        <v>328</v>
+      </c>
+      <c r="I71" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>388</v>
+        <v>352</v>
       </c>
       <c r="D72" t="s">
         <v>230</v>
       </c>
       <c r="E72" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="F72" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G72" s="6"/>
       <c r="H72" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I72" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B73" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="D73" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E73" t="s">
-        <v>234</v>
+        <v>171</v>
       </c>
       <c r="F73" t="s">
         <v>235</v>
       </c>
-      <c r="G73" s="5" t="s">
-        <v>354</v>
-      </c>
+      <c r="G73" s="5"/>
       <c r="H73" t="s">
-        <v>335</v>
-      </c>
-      <c r="I73" t="s">
-        <v>265</v>
+        <v>330</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
       <c r="C74" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
       <c r="D74" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E74" t="s">
-        <v>237</v>
+        <v>150</v>
       </c>
       <c r="F74" t="s">
         <v>238</v>
       </c>
-      <c r="G74" s="6"/>
+      <c r="G74" s="5" t="s">
+        <v>258</v>
+      </c>
       <c r="H74" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="I74" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B75" t="s">
         <v>239</v>
       </c>
       <c r="C75" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="D75" t="s">
         <v>240</v>
       </c>
       <c r="E75" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F75" t="s">
-        <v>241</v>
-      </c>
-      <c r="G75" s="5"/>
+        <v>242</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>338</v>
+      </c>
       <c r="H75" t="s">
-        <v>337</v>
+        <v>332</v>
+      </c>
+      <c r="I75" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B76" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C76" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
       <c r="D76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E76" t="s">
-        <v>156</v>
+        <v>245</v>
       </c>
       <c r="F76" t="s">
-        <v>244</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>264</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="G76" s="5"/>
       <c r="H76" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="I76" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C77" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="D77" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E77" t="s">
-        <v>247</v>
+        <v>44</v>
       </c>
       <c r="F77" t="s">
-        <v>248</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>346</v>
+        <v>249</v>
+      </c>
+      <c r="G77" s="5">
+        <v>37527191</v>
       </c>
       <c r="H77" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I77" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C78" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="D78" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E78" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F78" t="s">
-        <v>252</v>
-      </c>
-      <c r="G78" s="5"/>
+        <v>253</v>
+      </c>
+      <c r="G78" s="6"/>
       <c r="H78" t="s">
-        <v>340</v>
-      </c>
-      <c r="I78" t="s">
-        <v>265</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B79" t="s">
-        <v>253</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="D79" t="s">
         <v>254</v>
       </c>
       <c r="E79" t="s">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="F79" t="s">
-        <v>255</v>
-      </c>
-      <c r="G79" s="5">
-        <v>37527191</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="G79" s="5"/>
       <c r="H79" t="s">
-        <v>341</v>
-      </c>
-      <c r="I79" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>200</v>
-      </c>
-      <c r="B80" t="s">
-        <v>256</v>
-      </c>
-      <c r="C80" t="s">
-        <v>359</v>
-      </c>
-      <c r="D80" t="s">
-        <v>257</v>
-      </c>
-      <c r="E80" t="s">
-        <v>258</v>
-      </c>
-      <c r="F80" t="s">
-        <v>259</v>
-      </c>
-      <c r="G80" s="6"/>
-      <c r="H80" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>203</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
-        <v>401</v>
-      </c>
-      <c r="D81" t="s">
-        <v>260</v>
-      </c>
-      <c r="E81" t="s">
-        <v>261</v>
-      </c>
-      <c r="F81" t="s">
-        <v>262</v>
-      </c>
-      <c r="G81" s="5"/>
-      <c r="H81" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I81" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I81">
-      <sortCondition ref="A1:A81"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I79" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
add linked publication from additional search
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_AI_search_checked.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76564A0-A35A-C149-851F-183AD2A81540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6C17F-6956-604C-B500-661DA00F3BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="500" windowWidth="32160" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9060" yWindow="500" windowWidth="32160" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="420">
   <si>
     <t>RefID</t>
   </si>
@@ -1407,6 +1407,9 @@
   </si>
   <si>
     <t>DQ301502, DQ301503, DQ301504, DQ301505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.5812/archcid-129126 </t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1509,6 +1512,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1814,7 +1820,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1947,7 +1953,9 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5">
+        <v>19523314</v>
+      </c>
       <c r="H5" t="s">
         <v>264</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>53</v>
       </c>
@@ -2240,7 +2248,9 @@
       <c r="F17" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="7" t="s">
+        <v>419</v>
+      </c>
       <c r="H17" t="s">
         <v>276</v>
       </c>

</xml_diff>